<commit_message>
Some other editing (see previous review)
Former-commit-id: 2786f4dfa29e5724a3d3686cf3a22b2cad7e4955
</commit_message>
<xml_diff>
--- a/result_report.xlsx
+++ b/result_report.xlsx
@@ -263,8 +263,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -752,31 +752,27 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,7 +784,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -892,67 +888,16 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -976,19 +921,67 @@
     <xf numFmtId="11" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1296,96 +1289,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL106"/>
+  <dimension ref="A1:BM106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AT14" sqref="AT14"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AU9" sqref="AU9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="38" max="38" width="13" customWidth="1"/>
-    <col min="43" max="43" width="10.85546875" customWidth="1"/>
-    <col min="44" max="44" width="14" customWidth="1"/>
-    <col min="45" max="45" width="10.5703125" customWidth="1"/>
-    <col min="46" max="46" width="12" customWidth="1"/>
-    <col min="47" max="47" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.28515625" customWidth="1"/>
-    <col min="49" max="49" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.5703125" customWidth="1"/>
-    <col min="51" max="51" width="63.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="39" max="39" width="13" customWidth="1"/>
+    <col min="44" max="44" width="10.85546875" customWidth="1"/>
+    <col min="45" max="45" width="14" customWidth="1"/>
+    <col min="46" max="46" width="10.5703125" customWidth="1"/>
+    <col min="47" max="47" width="12" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.28515625" customWidth="1"/>
+    <col min="50" max="50" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.5703125" customWidth="1"/>
+    <col min="52" max="52" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:65" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="47" t="s">
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47"/>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="47"/>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="47"/>
-      <c r="AP1" s="47"/>
-      <c r="AQ1" s="67" t="s">
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="63"/>
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="63"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="67"/>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="40" t="s">
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="64"/>
+      <c r="AV1" s="64"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="AZ1" s="3"/>
       <c r="BA1" s="3"/>
       <c r="BB1" s="3"/>
-      <c r="BC1" s="1"/>
+      <c r="BC1" s="3"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
       <c r="BF1" s="1"/>
@@ -1395,91 +1388,92 @@
       <c r="BJ1" s="1"/>
       <c r="BK1" s="1"/>
       <c r="BL1" s="1"/>
-    </row>
-    <row r="2" spans="1:64" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="38" t="s">
+      <c r="BM1" s="1"/>
+    </row>
+    <row r="2" spans="1:65" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38" t="s">
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="41" t="s">
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="42"/>
-      <c r="AH2" s="43"/>
-      <c r="AI2" s="41" t="s">
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="53"/>
+      <c r="AJ2" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="AJ2" s="42"/>
-      <c r="AK2" s="43"/>
-      <c r="AL2" s="44" t="s">
+      <c r="AK2" s="52"/>
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="AM2" s="54" t="s">
+      <c r="AN2" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="AN2" s="55"/>
-      <c r="AO2" s="35" t="s">
+      <c r="AO2" s="60"/>
+      <c r="AP2" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="AP2" s="49" t="s">
+      <c r="AQ2" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="AQ2" s="41" t="s">
+      <c r="AR2" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="AR2" s="42"/>
-      <c r="AS2" s="42"/>
-      <c r="AT2" s="43"/>
-      <c r="AU2" s="41" t="s">
+      <c r="AS2" s="52"/>
+      <c r="AT2" s="52"/>
+      <c r="AU2" s="53"/>
+      <c r="AV2" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="AV2" s="42"/>
-      <c r="AW2" s="42"/>
-      <c r="AX2" s="43"/>
-      <c r="AY2" s="40"/>
-      <c r="AZ2" s="3"/>
+      <c r="AW2" s="52"/>
+      <c r="AX2" s="52"/>
+      <c r="AY2" s="53"/>
+      <c r="AZ2" s="56"/>
       <c r="BA2" s="3"/>
       <c r="BB2" s="3"/>
-      <c r="BC2" s="1"/>
+      <c r="BC2" s="3"/>
       <c r="BD2" s="1"/>
       <c r="BE2" s="1"/>
       <c r="BF2" s="1"/>
@@ -1489,9 +1483,10 @@
       <c r="BJ2" s="1"/>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
-    </row>
-    <row r="3" spans="1:64" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
+      <c r="BM2" s="1"/>
+    </row>
+    <row r="3" spans="1:65" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48"/>
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
@@ -1504,140 +1499,140 @@
       <c r="E3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="55"/>
+      <c r="H3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="P3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="Q3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="R3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="S3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="T3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="U3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="V3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="W3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="X3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="Y3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Z3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="AA3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AB3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AB3" s="15" t="s">
+      <c r="AC3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AC3" s="15" t="s">
+      <c r="AD3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AE3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AE3" s="15" t="s">
+      <c r="AF3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AF3" s="15" t="s">
+      <c r="AG3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AG3" s="15" t="s">
+      <c r="AH3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AH3" s="24" t="s">
+      <c r="AI3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AI3" s="15" t="s">
+      <c r="AJ3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="AJ3" s="15" t="s">
+      <c r="AK3" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AK3" s="15" t="s">
+      <c r="AL3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="45"/>
-      <c r="AM3" s="15" t="s">
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="AN3" s="15" t="s">
+      <c r="AO3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="AO3" s="36"/>
-      <c r="AP3" s="50"/>
-      <c r="AQ3" s="48" t="s">
+      <c r="AP3" s="66"/>
+      <c r="AQ3" s="62"/>
+      <c r="AR3" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="AR3" s="48" t="s">
+      <c r="AS3" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="AS3" s="48" t="s">
+      <c r="AT3" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="AT3" s="48" t="s">
+      <c r="AU3" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="AU3" s="48" t="s">
+      <c r="AV3" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="AV3" s="48" t="s">
+      <c r="AW3" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="AW3" s="48" t="s">
+      <c r="AX3" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="AX3" s="51" t="s">
+      <c r="AY3" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AY3" s="40"/>
-      <c r="AZ3" s="3"/>
+      <c r="AZ3" s="56"/>
       <c r="BA3" s="3"/>
       <c r="BB3" s="3"/>
-      <c r="BC3" s="1"/>
+      <c r="BC3" s="3"/>
       <c r="BD3" s="1"/>
       <c r="BE3" s="1"/>
       <c r="BF3" s="1"/>
@@ -1647,8 +1642,9 @@
       <c r="BJ3" s="1"/>
       <c r="BK3" s="1"/>
       <c r="BL3" s="1"/>
-    </row>
-    <row r="4" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BM3" s="1"/>
+    </row>
+    <row r="4" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
@@ -1664,156 +1660,158 @@
       <c r="E4" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="52">
-        <v>106.36</v>
-      </c>
-      <c r="G4" s="8">
+      <c r="F4" s="32">
+        <v>80.522000000000006</v>
+      </c>
+      <c r="G4" s="32">
+        <v>106.298</v>
+      </c>
+      <c r="H4" s="8">
         <v>80</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="8">
         <v>9904</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J4" s="8">
         <v>16889</v>
       </c>
-      <c r="J4" s="53">
+      <c r="K4" s="38">
         <v>2.4670000000000001</v>
       </c>
-      <c r="K4" s="53">
+      <c r="L4" s="38">
         <v>0.72099999999999997</v>
       </c>
-      <c r="L4" s="53">
+      <c r="M4" s="38">
         <v>3.1880000000000002</v>
       </c>
-      <c r="M4" s="63">
-        <f>L4/F4</f>
-        <v>2.9973674313651749E-2</v>
-      </c>
-      <c r="N4" s="29">
+      <c r="N4" s="46">
+        <f>M4/F4</f>
+        <v>3.9591664389856188E-2</v>
+      </c>
+      <c r="O4" s="29">
         <v>100</v>
       </c>
-      <c r="O4" s="29">
+      <c r="P4" s="29">
         <v>117</v>
       </c>
-      <c r="P4" s="29">
+      <c r="Q4" s="29">
         <v>67</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="R4" s="29">
         <v>100</v>
       </c>
-      <c r="R4" s="29">
+      <c r="S4" s="29">
         <v>816</v>
       </c>
-      <c r="S4" s="29">
+      <c r="T4" s="29">
         <v>717</v>
       </c>
-      <c r="T4" s="29">
+      <c r="U4" s="29">
         <v>83</v>
       </c>
-      <c r="U4" s="29">
+      <c r="V4" s="29">
         <v>150</v>
       </c>
-      <c r="V4" s="29">
+      <c r="W4" s="29">
         <v>417</v>
       </c>
-      <c r="W4" s="29">
+      <c r="X4" s="29">
         <v>1150</v>
       </c>
-      <c r="X4" s="29">
+      <c r="Y4" s="29">
         <v>253</v>
       </c>
-      <c r="Y4" s="29">
+      <c r="Z4" s="29">
         <v>1001</v>
       </c>
-      <c r="Z4" s="32" t="s">
+      <c r="AA4" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="AA4" s="32" t="s">
+      <c r="AB4" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" s="32" t="s">
+      <c r="AC4" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="AC4" s="32" t="s">
+      <c r="AD4" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AD4" s="32" t="s">
+      <c r="AE4" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="AE4" s="32" t="s">
+      <c r="AF4" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="32">
+      <c r="AG4" s="32">
         <v>1.6579999999999999</v>
       </c>
-      <c r="AG4" s="32">
+      <c r="AH4" s="32">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AH4" s="33">
+      <c r="AI4" s="33">
         <v>2.3849999999999998</v>
       </c>
-      <c r="AI4" s="25">
+      <c r="AJ4" s="25">
         <v>801</v>
       </c>
-      <c r="AJ4" s="29">
+      <c r="AK4" s="29">
         <v>16286</v>
       </c>
-      <c r="AK4" s="29">
+      <c r="AL4" s="29">
         <v>5257</v>
       </c>
-      <c r="AL4" s="25">
+      <c r="AM4" s="25">
         <v>7.86</v>
       </c>
-      <c r="AM4" s="25">
+      <c r="AN4" s="25">
         <v>20.5</v>
       </c>
-      <c r="AN4" s="25">
+      <c r="AO4" s="25">
         <v>20.57</v>
       </c>
-      <c r="AO4" s="25">
+      <c r="AP4" s="25">
         <v>9.84</v>
       </c>
-      <c r="AP4" s="25">
+      <c r="AQ4" s="25">
         <f>3*60+29.32</f>
         <v>209.32</v>
       </c>
-      <c r="AQ4" s="56">
-        <f>H4+I4</f>
+      <c r="AR4" s="39">
+        <f t="shared" ref="AR4:AR12" si="0">I4+J4</f>
         <v>26793</v>
       </c>
-      <c r="AR4" s="57">
+      <c r="AS4" s="40">
         <f>1/F4</f>
-        <v>9.4020308386611514E-3</v>
-      </c>
-      <c r="AS4" s="57">
-        <f>L4</f>
+        <v>1.2418966245249744E-2</v>
+      </c>
+      <c r="AT4" s="40">
+        <f t="shared" ref="AT4:AT12" si="1">M4</f>
         <v>3.1880000000000002</v>
       </c>
-      <c r="AT4" s="57">
-        <f>AP4</f>
+      <c r="AU4" s="40">
+        <f>AQ4</f>
         <v>209.32</v>
       </c>
-      <c r="AU4" s="58">
-        <f>AQ4*AR4</f>
-        <v>251.90861226024822</v>
-      </c>
-      <c r="AV4" s="57">
-        <f>AQ4*AT4</f>
+      <c r="AV4" s="41">
+        <f>AR4*AS4</f>
+        <v>332.74136260897637</v>
+      </c>
+      <c r="AW4" s="40">
+        <f>AR4*AU4</f>
         <v>5608310.7599999998</v>
       </c>
-      <c r="AW4" s="57">
-        <f>AS4*AR4</f>
-        <v>2.9973674313651753E-2</v>
-      </c>
-      <c r="AX4" s="59">
-        <f>AS4*AT4</f>
+      <c r="AX4" s="40">
+        <f>AT4*AS4</f>
+        <v>3.9591664389856188E-2</v>
+      </c>
+      <c r="AY4" s="42">
+        <f>AT4*AU4</f>
         <v>667.31216000000006</v>
       </c>
-      <c r="AY4" s="20"/>
-      <c r="AZ4" s="3"/>
+      <c r="AZ4" s="20"/>
       <c r="BA4" s="3"/>
       <c r="BB4" s="3"/>
-      <c r="BC4" s="1"/>
+      <c r="BC4" s="3"/>
       <c r="BD4" s="1"/>
       <c r="BE4" s="1"/>
       <c r="BF4" s="1"/>
@@ -1823,8 +1821,9 @@
       <c r="BJ4" s="1"/>
       <c r="BK4" s="1"/>
       <c r="BL4" s="1"/>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM4" s="1"/>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
@@ -1840,156 +1839,158 @@
       <c r="E5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="34">
+        <v>80.379000000000005</v>
+      </c>
+      <c r="G5" s="34">
         <v>106.39</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="10">
         <v>80</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="10">
         <v>10481</v>
       </c>
-      <c r="I5" s="10">
+      <c r="J5" s="10">
         <v>17915</v>
       </c>
-      <c r="J5" s="10">
+      <c r="K5" s="10">
         <v>2.468</v>
       </c>
-      <c r="K5" s="10">
+      <c r="L5" s="10">
         <v>0.74299999999999999</v>
       </c>
-      <c r="L5" s="10">
+      <c r="M5" s="10">
         <v>3.2109999999999999</v>
       </c>
-      <c r="M5" s="64">
-        <f t="shared" ref="M5:M12" si="0">L5/F5</f>
-        <v>3.0181408027070211E-2</v>
-      </c>
-      <c r="N5" s="30">
+      <c r="N5" s="46">
+        <f t="shared" ref="N5:N12" si="2">M5/F5</f>
+        <v>3.9948245188419856E-2</v>
+      </c>
+      <c r="O5" s="30">
         <v>100</v>
       </c>
-      <c r="O5" s="30">
+      <c r="P5" s="30">
         <v>117</v>
       </c>
-      <c r="P5" s="30">
+      <c r="Q5" s="30">
         <v>67</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="R5" s="30">
         <v>100</v>
       </c>
-      <c r="R5" s="30">
+      <c r="S5" s="30">
         <v>816</v>
       </c>
-      <c r="S5" s="30">
+      <c r="T5" s="30">
         <v>717</v>
       </c>
-      <c r="T5" s="30">
+      <c r="U5" s="30">
         <v>83</v>
       </c>
-      <c r="U5" s="30">
+      <c r="V5" s="30">
         <v>150</v>
       </c>
-      <c r="V5" s="30">
+      <c r="W5" s="30">
         <v>417</v>
       </c>
-      <c r="W5" s="30">
+      <c r="X5" s="30">
         <v>1150</v>
       </c>
-      <c r="X5" s="30">
+      <c r="Y5" s="30">
         <v>253</v>
       </c>
-      <c r="Y5" s="30">
+      <c r="Z5" s="30">
         <v>1001</v>
       </c>
-      <c r="Z5" s="34">
+      <c r="AA5" s="34">
         <v>0.45400000000000001</v>
       </c>
-      <c r="AA5" s="34">
+      <c r="AB5" s="34">
         <v>0.29099999999999998</v>
       </c>
-      <c r="AB5" s="34">
+      <c r="AC5" s="34">
         <v>0.27400000000000002</v>
       </c>
-      <c r="AC5" s="34">
+      <c r="AD5" s="34">
         <v>0.246</v>
       </c>
-      <c r="AD5" s="34">
+      <c r="AE5" s="34">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AE5" s="34">
+      <c r="AF5" s="34">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AF5" s="34">
+      <c r="AG5" s="34">
         <v>1.68</v>
       </c>
-      <c r="AG5" s="34">
+      <c r="AH5" s="34">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AH5" s="34">
+      <c r="AI5" s="34">
         <v>2.3849999999999998</v>
       </c>
-      <c r="AI5" s="27">
+      <c r="AJ5" s="27">
         <v>800</v>
       </c>
-      <c r="AJ5" s="30">
+      <c r="AK5" s="30">
         <v>16292</v>
       </c>
-      <c r="AK5" s="30">
+      <c r="AL5" s="30">
         <v>5258</v>
       </c>
-      <c r="AL5" s="27">
+      <c r="AM5" s="27">
         <v>7.86</v>
       </c>
-      <c r="AM5" s="27">
+      <c r="AN5" s="27">
         <v>20.66</v>
       </c>
-      <c r="AN5" s="27">
+      <c r="AO5" s="27">
         <v>20.52</v>
       </c>
-      <c r="AO5" s="27">
+      <c r="AP5" s="27">
         <v>9.75</v>
       </c>
-      <c r="AP5" s="27">
+      <c r="AQ5" s="27">
         <f>3*60+28.7</f>
         <v>208.7</v>
       </c>
-      <c r="AQ5" s="56">
-        <f>H5+I5</f>
+      <c r="AR5" s="39">
+        <f t="shared" si="0"/>
         <v>28396</v>
       </c>
-      <c r="AR5" s="57">
-        <f>1/F5</f>
-        <v>9.3993796409436985E-3</v>
-      </c>
-      <c r="AS5" s="57">
-        <f>L5</f>
+      <c r="AS5" s="40">
+        <f t="shared" ref="AS5:AS12" si="3">1/F5</f>
+        <v>1.2441060475994973E-2</v>
+      </c>
+      <c r="AT5" s="40">
+        <f t="shared" si="1"/>
         <v>3.2109999999999999</v>
       </c>
-      <c r="AT5" s="57">
-        <f t="shared" ref="AT5:AT12" si="1">AP5</f>
+      <c r="AU5" s="40">
+        <f t="shared" ref="AU5:AU12" si="4">AQ5</f>
         <v>208.7</v>
       </c>
-      <c r="AU5" s="56">
-        <f t="shared" ref="AU5:AU12" si="2">AQ5*AR5</f>
-        <v>266.90478428423728</v>
-      </c>
-      <c r="AV5" s="57">
-        <f t="shared" ref="AV5:AV12" si="3">AQ5*AT5</f>
+      <c r="AV5" s="39">
+        <f t="shared" ref="AV5:AV12" si="5">AR5*AS5</f>
+        <v>353.27635327635323</v>
+      </c>
+      <c r="AW5" s="40">
+        <f t="shared" ref="AW5:AW12" si="6">AR5*AU5</f>
         <v>5926245.1999999993</v>
       </c>
-      <c r="AW5" s="57">
-        <f t="shared" ref="AW5:AW12" si="4">AS5*AR5</f>
-        <v>3.0181408027070214E-2</v>
-      </c>
-      <c r="AX5" s="59">
-        <f t="shared" ref="AX5:AX12" si="5">AS5*AT5</f>
+      <c r="AX5" s="40">
+        <f t="shared" ref="AX5:AX12" si="7">AT5*AS5</f>
+        <v>3.9948245188419856E-2</v>
+      </c>
+      <c r="AY5" s="42">
+        <f t="shared" ref="AY5:AY12" si="8">AT5*AU5</f>
         <v>670.13569999999993</v>
       </c>
-      <c r="AY5" s="21"/>
-      <c r="AZ5" s="3"/>
+      <c r="AZ5" s="21"/>
       <c r="BA5" s="3"/>
       <c r="BB5" s="3"/>
-      <c r="BC5" s="1"/>
+      <c r="BC5" s="3"/>
       <c r="BD5" s="1"/>
       <c r="BE5" s="1"/>
       <c r="BF5" s="1"/>
@@ -1999,8 +2000,9 @@
       <c r="BJ5" s="1"/>
       <c r="BK5" s="1"/>
       <c r="BL5" s="1"/>
-    </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM5" s="1"/>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>62</v>
       </c>
@@ -2016,156 +2018,158 @@
       <c r="E6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="33">
+        <v>80.483000000000004</v>
+      </c>
+      <c r="G6" s="33">
         <v>106.32899999999999</v>
       </c>
-      <c r="G6" s="12">
+      <c r="H6" s="12">
         <v>80</v>
       </c>
-      <c r="H6" s="12">
+      <c r="I6" s="12">
         <v>10468</v>
       </c>
-      <c r="I6" s="12">
+      <c r="J6" s="12">
         <v>17894</v>
       </c>
-      <c r="J6" s="12">
+      <c r="K6" s="12">
         <v>2.4689999999999999</v>
       </c>
-      <c r="K6" s="12">
+      <c r="L6" s="12">
         <v>0.75800000000000001</v>
       </c>
-      <c r="L6" s="12">
+      <c r="M6" s="12">
         <v>3.2269999999999999</v>
       </c>
-      <c r="M6" s="64">
-        <f t="shared" si="0"/>
-        <v>3.0349199183665791E-2</v>
-      </c>
-      <c r="N6" s="31">
+      <c r="N6" s="46">
+        <f t="shared" si="2"/>
+        <v>4.0095423878334549E-2</v>
+      </c>
+      <c r="O6" s="31">
         <v>100</v>
       </c>
-      <c r="O6" s="31">
+      <c r="P6" s="31">
         <v>117</v>
       </c>
-      <c r="P6" s="31">
+      <c r="Q6" s="31">
         <v>67</v>
       </c>
-      <c r="Q6" s="31">
+      <c r="R6" s="31">
         <v>100</v>
       </c>
-      <c r="R6" s="31">
+      <c r="S6" s="31">
         <v>816</v>
       </c>
-      <c r="S6" s="31">
+      <c r="T6" s="31">
         <v>717</v>
       </c>
-      <c r="T6" s="31">
+      <c r="U6" s="31">
         <v>83</v>
       </c>
-      <c r="U6" s="31">
+      <c r="V6" s="31">
         <v>150</v>
       </c>
-      <c r="V6" s="31">
+      <c r="W6" s="31">
         <v>434</v>
       </c>
-      <c r="W6" s="31">
+      <c r="X6" s="31">
         <v>1150</v>
       </c>
-      <c r="X6" s="31">
+      <c r="Y6" s="31">
         <v>257</v>
       </c>
-      <c r="Y6" s="31">
+      <c r="Z6" s="31">
         <v>1006</v>
       </c>
-      <c r="Z6" s="33">
+      <c r="AA6" s="33">
         <v>0.45400000000000001</v>
       </c>
-      <c r="AA6" s="33">
+      <c r="AB6" s="33">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AB6" s="33">
+      <c r="AC6" s="33">
         <v>0.27400000000000002</v>
       </c>
-      <c r="AC6" s="33">
+      <c r="AD6" s="33">
         <v>0.246</v>
       </c>
-      <c r="AD6" s="33">
+      <c r="AE6" s="33">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AE6" s="33">
+      <c r="AF6" s="33">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AF6" s="33">
+      <c r="AG6" s="33">
         <v>1.68</v>
       </c>
-      <c r="AG6" s="33">
+      <c r="AH6" s="33">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AH6" s="33">
+      <c r="AI6" s="33">
         <v>2.3839999999999999</v>
       </c>
-      <c r="AI6" s="26">
+      <c r="AJ6" s="26">
         <v>801</v>
       </c>
-      <c r="AJ6" s="31">
+      <c r="AK6" s="31">
         <v>16286</v>
       </c>
-      <c r="AK6" s="31">
+      <c r="AL6" s="31">
         <v>5257</v>
       </c>
-      <c r="AL6" s="26">
+      <c r="AM6" s="26">
         <v>7.86</v>
       </c>
-      <c r="AM6" s="26">
+      <c r="AN6" s="26">
         <v>20.53</v>
       </c>
-      <c r="AN6" s="26">
+      <c r="AO6" s="26">
         <v>20.41</v>
       </c>
-      <c r="AO6" s="26">
+      <c r="AP6" s="26">
         <v>9.85</v>
       </c>
-      <c r="AP6" s="26">
+      <c r="AQ6" s="26">
         <f>3*60+29.23</f>
         <v>209.23</v>
       </c>
-      <c r="AQ6" s="56">
-        <f>H6+I6</f>
+      <c r="AR6" s="39">
+        <f t="shared" si="0"/>
         <v>28362</v>
       </c>
-      <c r="AR6" s="57">
-        <f>1/F6</f>
-        <v>9.4047719813033139E-3</v>
-      </c>
-      <c r="AS6" s="57">
-        <f>L6</f>
+      <c r="AS6" s="40">
+        <f t="shared" si="3"/>
+        <v>1.2424984158145198E-2</v>
+      </c>
+      <c r="AT6" s="40">
+        <f t="shared" si="1"/>
         <v>3.2269999999999999</v>
       </c>
-      <c r="AT6" s="57">
-        <f t="shared" si="1"/>
+      <c r="AU6" s="40">
+        <f t="shared" si="4"/>
         <v>209.23</v>
       </c>
-      <c r="AU6" s="56">
-        <f t="shared" si="2"/>
-        <v>266.73814293372459</v>
-      </c>
-      <c r="AV6" s="57">
-        <f t="shared" si="3"/>
+      <c r="AV6" s="39">
+        <f t="shared" si="5"/>
+        <v>352.39740069331413</v>
+      </c>
+      <c r="AW6" s="40">
+        <f t="shared" si="6"/>
         <v>5934181.2599999998</v>
       </c>
-      <c r="AW6" s="57">
-        <f t="shared" si="4"/>
-        <v>3.0349199183665791E-2</v>
-      </c>
-      <c r="AX6" s="59">
-        <f t="shared" si="5"/>
+      <c r="AX6" s="40">
+        <f t="shared" si="7"/>
+        <v>4.0095423878334556E-2</v>
+      </c>
+      <c r="AY6" s="42">
+        <f t="shared" si="8"/>
         <v>675.18520999999998</v>
       </c>
-      <c r="AY6" s="22"/>
-      <c r="AZ6" s="3"/>
+      <c r="AZ6" s="22"/>
       <c r="BA6" s="3"/>
       <c r="BB6" s="3"/>
-      <c r="BC6" s="1"/>
+      <c r="BC6" s="3"/>
       <c r="BD6" s="1"/>
       <c r="BE6" s="1"/>
       <c r="BF6" s="1"/>
@@ -2175,8 +2179,9 @@
       <c r="BJ6" s="1"/>
       <c r="BK6" s="1"/>
       <c r="BL6" s="1"/>
-    </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM6" s="1"/>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
@@ -2189,11 +2194,11 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="65" t="e">
-        <f t="shared" si="0"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="46" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" s="27"/>
       <c r="O7" s="27"/>
       <c r="P7" s="27"/>
       <c r="Q7" s="27"/>
@@ -2222,43 +2227,43 @@
       <c r="AN7" s="27"/>
       <c r="AO7" s="27"/>
       <c r="AP7" s="27"/>
-      <c r="AQ7" s="56">
-        <f>H7+I7</f>
+      <c r="AQ7" s="27"/>
+      <c r="AR7" s="39">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR7" s="57" t="e">
-        <f>1/F7</f>
+      <c r="AS7" s="40" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS7" s="57">
-        <f>L7</f>
-        <v>0</v>
-      </c>
-      <c r="AT7" s="57">
+      <c r="AT7" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU7" s="56" t="e">
-        <f t="shared" si="2"/>
+      <c r="AU7" s="40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV7" s="39" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AV7" s="57">
-        <f t="shared" si="3"/>
+      <c r="AW7" s="40">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AW7" s="57" t="e">
-        <f t="shared" si="4"/>
+      <c r="AX7" s="40" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX7" s="59">
-        <f t="shared" si="5"/>
+      <c r="AY7" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AY7" s="21"/>
-      <c r="AZ7" s="3"/>
+      <c r="AZ7" s="21"/>
       <c r="BA7" s="3"/>
       <c r="BB7" s="3"/>
-      <c r="BC7" s="1"/>
+      <c r="BC7" s="3"/>
       <c r="BD7" s="1"/>
       <c r="BE7" s="1"/>
       <c r="BF7" s="1"/>
@@ -2268,8 +2273,9 @@
       <c r="BJ7" s="1"/>
       <c r="BK7" s="1"/>
       <c r="BL7" s="1"/>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM7" s="1"/>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -2282,11 +2288,11 @@
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
-      <c r="M8" s="65" t="e">
-        <f t="shared" si="0"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="46" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N8" s="26"/>
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
       <c r="Q8" s="26"/>
@@ -2315,43 +2321,43 @@
       <c r="AN8" s="26"/>
       <c r="AO8" s="26"/>
       <c r="AP8" s="26"/>
-      <c r="AQ8" s="56">
-        <f>H8+I8</f>
+      <c r="AQ8" s="26"/>
+      <c r="AR8" s="39">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR8" s="57" t="e">
-        <f>1/F8</f>
+      <c r="AS8" s="40" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS8" s="57">
-        <f>L8</f>
-        <v>0</v>
-      </c>
-      <c r="AT8" s="57">
+      <c r="AT8" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU8" s="56" t="e">
-        <f t="shared" si="2"/>
+      <c r="AU8" s="40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV8" s="39" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AV8" s="57">
-        <f t="shared" si="3"/>
+      <c r="AW8" s="40">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AW8" s="57" t="e">
-        <f t="shared" si="4"/>
+      <c r="AX8" s="40" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX8" s="59">
-        <f t="shared" si="5"/>
+      <c r="AY8" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AY8" s="22"/>
-      <c r="AZ8" s="3"/>
+      <c r="AZ8" s="22"/>
       <c r="BA8" s="3"/>
       <c r="BB8" s="3"/>
-      <c r="BC8" s="1"/>
+      <c r="BC8" s="3"/>
       <c r="BD8" s="1"/>
       <c r="BE8" s="1"/>
       <c r="BF8" s="1"/>
@@ -2361,8 +2367,9 @@
       <c r="BJ8" s="1"/>
       <c r="BK8" s="1"/>
       <c r="BL8" s="1"/>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM8" s="1"/>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -2375,11 +2382,11 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="65" t="e">
-        <f t="shared" si="0"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="46" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" s="27"/>
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
       <c r="Q9" s="27"/>
@@ -2408,43 +2415,43 @@
       <c r="AN9" s="27"/>
       <c r="AO9" s="27"/>
       <c r="AP9" s="27"/>
-      <c r="AQ9" s="56">
-        <f>H9+I9</f>
+      <c r="AQ9" s="27"/>
+      <c r="AR9" s="39">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR9" s="57" t="e">
-        <f>1/F9</f>
+      <c r="AS9" s="40" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS9" s="57">
-        <f>L9</f>
-        <v>0</v>
-      </c>
-      <c r="AT9" s="57">
+      <c r="AT9" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU9" s="56" t="e">
-        <f t="shared" si="2"/>
+      <c r="AU9" s="40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV9" s="39" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AV9" s="57">
-        <f t="shared" si="3"/>
+      <c r="AW9" s="40">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AW9" s="57" t="e">
-        <f t="shared" si="4"/>
+      <c r="AX9" s="40" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX9" s="59">
-        <f t="shared" si="5"/>
+      <c r="AY9" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AY9" s="21"/>
-      <c r="AZ9" s="3"/>
+      <c r="AZ9" s="21"/>
       <c r="BA9" s="3"/>
       <c r="BB9" s="3"/>
-      <c r="BC9" s="1"/>
+      <c r="BC9" s="3"/>
       <c r="BD9" s="1"/>
       <c r="BE9" s="1"/>
       <c r="BF9" s="1"/>
@@ -2454,8 +2461,9 @@
       <c r="BJ9" s="1"/>
       <c r="BK9" s="1"/>
       <c r="BL9" s="1"/>
-    </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM9" s="1"/>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
@@ -2468,11 +2476,11 @@
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
-      <c r="M10" s="65" t="e">
-        <f t="shared" si="0"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="46" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="26"/>
       <c r="O10" s="26"/>
       <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
@@ -2501,43 +2509,43 @@
       <c r="AN10" s="26"/>
       <c r="AO10" s="26"/>
       <c r="AP10" s="26"/>
-      <c r="AQ10" s="56">
-        <f>H10+I10</f>
+      <c r="AQ10" s="26"/>
+      <c r="AR10" s="39">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR10" s="57" t="e">
-        <f>1/F10</f>
+      <c r="AS10" s="40" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS10" s="57">
-        <f>L10</f>
-        <v>0</v>
-      </c>
-      <c r="AT10" s="57">
+      <c r="AT10" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU10" s="56" t="e">
-        <f t="shared" si="2"/>
+      <c r="AU10" s="40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV10" s="39" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AV10" s="57">
-        <f t="shared" si="3"/>
+      <c r="AW10" s="40">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AW10" s="57" t="e">
-        <f t="shared" si="4"/>
+      <c r="AX10" s="40" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX10" s="59">
-        <f t="shared" si="5"/>
+      <c r="AY10" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AY10" s="22"/>
-      <c r="AZ10" s="3"/>
+      <c r="AZ10" s="22"/>
       <c r="BA10" s="3"/>
       <c r="BB10" s="3"/>
-      <c r="BC10" s="1"/>
+      <c r="BC10" s="3"/>
       <c r="BD10" s="1"/>
       <c r="BE10" s="1"/>
       <c r="BF10" s="1"/>
@@ -2547,8 +2555,9 @@
       <c r="BJ10" s="1"/>
       <c r="BK10" s="1"/>
       <c r="BL10" s="1"/>
-    </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM10" s="1"/>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -2561,11 +2570,11 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="65" t="e">
-        <f t="shared" si="0"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="46" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N11" s="27"/>
       <c r="O11" s="27"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
@@ -2594,43 +2603,43 @@
       <c r="AN11" s="27"/>
       <c r="AO11" s="27"/>
       <c r="AP11" s="27"/>
-      <c r="AQ11" s="56">
-        <f>H11+I11</f>
+      <c r="AQ11" s="27"/>
+      <c r="AR11" s="39">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR11" s="57" t="e">
-        <f>1/F11</f>
+      <c r="AS11" s="40" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS11" s="57">
-        <f>L11</f>
-        <v>0</v>
-      </c>
-      <c r="AT11" s="57">
+      <c r="AT11" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU11" s="56" t="e">
-        <f t="shared" si="2"/>
+      <c r="AU11" s="40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV11" s="39" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AV11" s="57">
-        <f t="shared" si="3"/>
+      <c r="AW11" s="40">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AW11" s="57" t="e">
-        <f t="shared" si="4"/>
+      <c r="AX11" s="40" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX11" s="59">
-        <f t="shared" si="5"/>
+      <c r="AY11" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AY11" s="21"/>
-      <c r="AZ11" s="3"/>
+      <c r="AZ11" s="21"/>
       <c r="BA11" s="3"/>
       <c r="BB11" s="3"/>
-      <c r="BC11" s="1"/>
+      <c r="BC11" s="3"/>
       <c r="BD11" s="1"/>
       <c r="BE11" s="1"/>
       <c r="BF11" s="1"/>
@@ -2640,8 +2649,9 @@
       <c r="BJ11" s="1"/>
       <c r="BK11" s="1"/>
       <c r="BL11" s="1"/>
-    </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM11" s="1"/>
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
@@ -2654,11 +2664,11 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="66" t="e">
-        <f t="shared" si="0"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="46" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N12" s="28"/>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="28"/>
@@ -2687,43 +2697,43 @@
       <c r="AN12" s="28"/>
       <c r="AO12" s="28"/>
       <c r="AP12" s="28"/>
-      <c r="AQ12" s="60">
-        <f>H12+I12</f>
+      <c r="AQ12" s="28"/>
+      <c r="AR12" s="43">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AR12" s="61" t="e">
-        <f>1/F12</f>
+      <c r="AS12" s="44" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS12" s="61">
-        <f>L12</f>
-        <v>0</v>
-      </c>
-      <c r="AT12" s="61">
+      <c r="AT12" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU12" s="60" t="e">
-        <f t="shared" si="2"/>
+      <c r="AU12" s="44">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV12" s="43" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AV12" s="61">
-        <f t="shared" si="3"/>
+      <c r="AW12" s="44">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AW12" s="61" t="e">
-        <f t="shared" si="4"/>
+      <c r="AX12" s="44" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AX12" s="62">
-        <f t="shared" si="5"/>
+      <c r="AY12" s="45">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AY12" s="23"/>
-      <c r="AZ12" s="3"/>
+      <c r="AZ12" s="23"/>
       <c r="BA12" s="3"/>
       <c r="BB12" s="3"/>
-      <c r="BC12" s="1"/>
+      <c r="BC12" s="3"/>
       <c r="BD12" s="1"/>
       <c r="BE12" s="1"/>
       <c r="BF12" s="1"/>
@@ -2733,8 +2743,9 @@
       <c r="BJ12" s="1"/>
       <c r="BK12" s="1"/>
       <c r="BL12" s="1"/>
-    </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM12" s="1"/>
+    </row>
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2789,7 +2800,7 @@
       <c r="AZ13" s="3"/>
       <c r="BA13" s="3"/>
       <c r="BB13" s="3"/>
-      <c r="BC13" s="1"/>
+      <c r="BC13" s="3"/>
       <c r="BD13" s="1"/>
       <c r="BE13" s="1"/>
       <c r="BF13" s="1"/>
@@ -2799,8 +2810,9 @@
       <c r="BJ13" s="1"/>
       <c r="BK13" s="1"/>
       <c r="BL13" s="1"/>
-    </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM13" s="1"/>
+    </row>
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2855,7 +2867,7 @@
       <c r="AZ14" s="3"/>
       <c r="BA14" s="3"/>
       <c r="BB14" s="3"/>
-      <c r="BC14" s="1"/>
+      <c r="BC14" s="3"/>
       <c r="BD14" s="1"/>
       <c r="BE14" s="1"/>
       <c r="BF14" s="1"/>
@@ -2865,8 +2877,9 @@
       <c r="BJ14" s="1"/>
       <c r="BK14" s="1"/>
       <c r="BL14" s="1"/>
-    </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM14" s="1"/>
+    </row>
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2921,7 +2934,7 @@
       <c r="AZ15" s="3"/>
       <c r="BA15" s="3"/>
       <c r="BB15" s="3"/>
-      <c r="BC15" s="1"/>
+      <c r="BC15" s="3"/>
       <c r="BD15" s="1"/>
       <c r="BE15" s="1"/>
       <c r="BF15" s="1"/>
@@ -2931,8 +2944,9 @@
       <c r="BJ15" s="1"/>
       <c r="BK15" s="1"/>
       <c r="BL15" s="1"/>
-    </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM15" s="1"/>
+    </row>
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2987,7 +3001,7 @@
       <c r="AZ16" s="3"/>
       <c r="BA16" s="3"/>
       <c r="BB16" s="3"/>
-      <c r="BC16" s="1"/>
+      <c r="BC16" s="3"/>
       <c r="BD16" s="1"/>
       <c r="BE16" s="1"/>
       <c r="BF16" s="1"/>
@@ -2997,8 +3011,9 @@
       <c r="BJ16" s="1"/>
       <c r="BK16" s="1"/>
       <c r="BL16" s="1"/>
-    </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM16" s="1"/>
+    </row>
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3053,7 +3068,7 @@
       <c r="AZ17" s="3"/>
       <c r="BA17" s="3"/>
       <c r="BB17" s="3"/>
-      <c r="BC17" s="1"/>
+      <c r="BC17" s="3"/>
       <c r="BD17" s="1"/>
       <c r="BE17" s="1"/>
       <c r="BF17" s="1"/>
@@ -3063,8 +3078,9 @@
       <c r="BJ17" s="1"/>
       <c r="BK17" s="1"/>
       <c r="BL17" s="1"/>
-    </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM17" s="1"/>
+    </row>
+    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3119,7 +3135,7 @@
       <c r="AZ18" s="3"/>
       <c r="BA18" s="3"/>
       <c r="BB18" s="3"/>
-      <c r="BC18" s="1"/>
+      <c r="BC18" s="3"/>
       <c r="BD18" s="1"/>
       <c r="BE18" s="1"/>
       <c r="BF18" s="1"/>
@@ -3129,8 +3145,9 @@
       <c r="BJ18" s="1"/>
       <c r="BK18" s="1"/>
       <c r="BL18" s="1"/>
-    </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM18" s="1"/>
+    </row>
+    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -3185,7 +3202,7 @@
       <c r="AZ19" s="3"/>
       <c r="BA19" s="3"/>
       <c r="BB19" s="3"/>
-      <c r="BC19" s="1"/>
+      <c r="BC19" s="3"/>
       <c r="BD19" s="1"/>
       <c r="BE19" s="1"/>
       <c r="BF19" s="1"/>
@@ -3195,8 +3212,9 @@
       <c r="BJ19" s="1"/>
       <c r="BK19" s="1"/>
       <c r="BL19" s="1"/>
-    </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM19" s="1"/>
+    </row>
+    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -3251,7 +3269,7 @@
       <c r="AZ20" s="3"/>
       <c r="BA20" s="3"/>
       <c r="BB20" s="3"/>
-      <c r="BC20" s="1"/>
+      <c r="BC20" s="3"/>
       <c r="BD20" s="1"/>
       <c r="BE20" s="1"/>
       <c r="BF20" s="1"/>
@@ -3261,8 +3279,9 @@
       <c r="BJ20" s="1"/>
       <c r="BK20" s="1"/>
       <c r="BL20" s="1"/>
-    </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM20" s="1"/>
+    </row>
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3317,7 +3336,7 @@
       <c r="AZ21" s="3"/>
       <c r="BA21" s="3"/>
       <c r="BB21" s="3"/>
-      <c r="BC21" s="1"/>
+      <c r="BC21" s="3"/>
       <c r="BD21" s="1"/>
       <c r="BE21" s="1"/>
       <c r="BF21" s="1"/>
@@ -3327,8 +3346,9 @@
       <c r="BJ21" s="1"/>
       <c r="BK21" s="1"/>
       <c r="BL21" s="1"/>
-    </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM21" s="1"/>
+    </row>
+    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3383,7 +3403,7 @@
       <c r="AZ22" s="3"/>
       <c r="BA22" s="3"/>
       <c r="BB22" s="3"/>
-      <c r="BC22" s="1"/>
+      <c r="BC22" s="3"/>
       <c r="BD22" s="1"/>
       <c r="BE22" s="1"/>
       <c r="BF22" s="1"/>
@@ -3393,8 +3413,9 @@
       <c r="BJ22" s="1"/>
       <c r="BK22" s="1"/>
       <c r="BL22" s="1"/>
-    </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM22" s="1"/>
+    </row>
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -3449,7 +3470,7 @@
       <c r="AZ23" s="3"/>
       <c r="BA23" s="3"/>
       <c r="BB23" s="3"/>
-      <c r="BC23" s="1"/>
+      <c r="BC23" s="3"/>
       <c r="BD23" s="1"/>
       <c r="BE23" s="1"/>
       <c r="BF23" s="1"/>
@@ -3459,8 +3480,9 @@
       <c r="BJ23" s="1"/>
       <c r="BK23" s="1"/>
       <c r="BL23" s="1"/>
-    </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM23" s="1"/>
+    </row>
+    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3515,7 +3537,7 @@
       <c r="AZ24" s="3"/>
       <c r="BA24" s="3"/>
       <c r="BB24" s="3"/>
-      <c r="BC24" s="1"/>
+      <c r="BC24" s="3"/>
       <c r="BD24" s="1"/>
       <c r="BE24" s="1"/>
       <c r="BF24" s="1"/>
@@ -3525,8 +3547,9 @@
       <c r="BJ24" s="1"/>
       <c r="BK24" s="1"/>
       <c r="BL24" s="1"/>
-    </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM24" s="1"/>
+    </row>
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -3581,7 +3604,7 @@
       <c r="AZ25" s="3"/>
       <c r="BA25" s="3"/>
       <c r="BB25" s="3"/>
-      <c r="BC25" s="1"/>
+      <c r="BC25" s="3"/>
       <c r="BD25" s="1"/>
       <c r="BE25" s="1"/>
       <c r="BF25" s="1"/>
@@ -3591,8 +3614,9 @@
       <c r="BJ25" s="1"/>
       <c r="BK25" s="1"/>
       <c r="BL25" s="1"/>
-    </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM25" s="1"/>
+    </row>
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3647,7 +3671,7 @@
       <c r="AZ26" s="3"/>
       <c r="BA26" s="3"/>
       <c r="BB26" s="3"/>
-      <c r="BC26" s="1"/>
+      <c r="BC26" s="3"/>
       <c r="BD26" s="1"/>
       <c r="BE26" s="1"/>
       <c r="BF26" s="1"/>
@@ -3657,8 +3681,9 @@
       <c r="BJ26" s="1"/>
       <c r="BK26" s="1"/>
       <c r="BL26" s="1"/>
-    </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM26" s="1"/>
+    </row>
+    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3713,7 +3738,7 @@
       <c r="AZ27" s="3"/>
       <c r="BA27" s="3"/>
       <c r="BB27" s="3"/>
-      <c r="BC27" s="1"/>
+      <c r="BC27" s="3"/>
       <c r="BD27" s="1"/>
       <c r="BE27" s="1"/>
       <c r="BF27" s="1"/>
@@ -3723,8 +3748,9 @@
       <c r="BJ27" s="1"/>
       <c r="BK27" s="1"/>
       <c r="BL27" s="1"/>
-    </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM27" s="1"/>
+    </row>
+    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3779,7 +3805,7 @@
       <c r="AZ28" s="3"/>
       <c r="BA28" s="3"/>
       <c r="BB28" s="3"/>
-      <c r="BC28" s="1"/>
+      <c r="BC28" s="3"/>
       <c r="BD28" s="1"/>
       <c r="BE28" s="1"/>
       <c r="BF28" s="1"/>
@@ -3789,8 +3815,9 @@
       <c r="BJ28" s="1"/>
       <c r="BK28" s="1"/>
       <c r="BL28" s="1"/>
-    </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM28" s="1"/>
+    </row>
+    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -3845,7 +3872,7 @@
       <c r="AZ29" s="3"/>
       <c r="BA29" s="3"/>
       <c r="BB29" s="3"/>
-      <c r="BC29" s="1"/>
+      <c r="BC29" s="3"/>
       <c r="BD29" s="1"/>
       <c r="BE29" s="1"/>
       <c r="BF29" s="1"/>
@@ -3855,8 +3882,9 @@
       <c r="BJ29" s="1"/>
       <c r="BK29" s="1"/>
       <c r="BL29" s="1"/>
-    </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM29" s="1"/>
+    </row>
+    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3911,7 +3939,7 @@
       <c r="AZ30" s="3"/>
       <c r="BA30" s="3"/>
       <c r="BB30" s="3"/>
-      <c r="BC30" s="1"/>
+      <c r="BC30" s="3"/>
       <c r="BD30" s="1"/>
       <c r="BE30" s="1"/>
       <c r="BF30" s="1"/>
@@ -3921,8 +3949,9 @@
       <c r="BJ30" s="1"/>
       <c r="BK30" s="1"/>
       <c r="BL30" s="1"/>
-    </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM30" s="1"/>
+    </row>
+    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -3977,7 +4006,7 @@
       <c r="AZ31" s="3"/>
       <c r="BA31" s="3"/>
       <c r="BB31" s="3"/>
-      <c r="BC31" s="1"/>
+      <c r="BC31" s="3"/>
       <c r="BD31" s="1"/>
       <c r="BE31" s="1"/>
       <c r="BF31" s="1"/>
@@ -3987,8 +4016,9 @@
       <c r="BJ31" s="1"/>
       <c r="BK31" s="1"/>
       <c r="BL31" s="1"/>
-    </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM31" s="1"/>
+    </row>
+    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4043,7 +4073,7 @@
       <c r="AZ32" s="3"/>
       <c r="BA32" s="3"/>
       <c r="BB32" s="3"/>
-      <c r="BC32" s="1"/>
+      <c r="BC32" s="3"/>
       <c r="BD32" s="1"/>
       <c r="BE32" s="1"/>
       <c r="BF32" s="1"/>
@@ -4053,8 +4083,9 @@
       <c r="BJ32" s="1"/>
       <c r="BK32" s="1"/>
       <c r="BL32" s="1"/>
-    </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM32" s="1"/>
+    </row>
+    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4109,7 +4140,7 @@
       <c r="AZ33" s="3"/>
       <c r="BA33" s="3"/>
       <c r="BB33" s="3"/>
-      <c r="BC33" s="1"/>
+      <c r="BC33" s="3"/>
       <c r="BD33" s="1"/>
       <c r="BE33" s="1"/>
       <c r="BF33" s="1"/>
@@ -4119,8 +4150,9 @@
       <c r="BJ33" s="1"/>
       <c r="BK33" s="1"/>
       <c r="BL33" s="1"/>
-    </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM33" s="1"/>
+    </row>
+    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4175,7 +4207,7 @@
       <c r="AZ34" s="3"/>
       <c r="BA34" s="3"/>
       <c r="BB34" s="3"/>
-      <c r="BC34" s="1"/>
+      <c r="BC34" s="3"/>
       <c r="BD34" s="1"/>
       <c r="BE34" s="1"/>
       <c r="BF34" s="1"/>
@@ -4185,8 +4217,9 @@
       <c r="BJ34" s="1"/>
       <c r="BK34" s="1"/>
       <c r="BL34" s="1"/>
-    </row>
-    <row r="35" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM34" s="1"/>
+    </row>
+    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4241,7 +4274,7 @@
       <c r="AZ35" s="3"/>
       <c r="BA35" s="3"/>
       <c r="BB35" s="3"/>
-      <c r="BC35" s="1"/>
+      <c r="BC35" s="3"/>
       <c r="BD35" s="1"/>
       <c r="BE35" s="1"/>
       <c r="BF35" s="1"/>
@@ -4251,8 +4284,9 @@
       <c r="BJ35" s="1"/>
       <c r="BK35" s="1"/>
       <c r="BL35" s="1"/>
-    </row>
-    <row r="36" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM35" s="1"/>
+    </row>
+    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4307,7 +4341,7 @@
       <c r="AZ36" s="3"/>
       <c r="BA36" s="3"/>
       <c r="BB36" s="3"/>
-      <c r="BC36" s="1"/>
+      <c r="BC36" s="3"/>
       <c r="BD36" s="1"/>
       <c r="BE36" s="1"/>
       <c r="BF36" s="1"/>
@@ -4317,8 +4351,9 @@
       <c r="BJ36" s="1"/>
       <c r="BK36" s="1"/>
       <c r="BL36" s="1"/>
-    </row>
-    <row r="37" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM36" s="1"/>
+    </row>
+    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4373,7 +4408,7 @@
       <c r="AZ37" s="3"/>
       <c r="BA37" s="3"/>
       <c r="BB37" s="3"/>
-      <c r="BC37" s="1"/>
+      <c r="BC37" s="3"/>
       <c r="BD37" s="1"/>
       <c r="BE37" s="1"/>
       <c r="BF37" s="1"/>
@@ -4383,8 +4418,9 @@
       <c r="BJ37" s="1"/>
       <c r="BK37" s="1"/>
       <c r="BL37" s="1"/>
-    </row>
-    <row r="38" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM37" s="1"/>
+    </row>
+    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4439,7 +4475,7 @@
       <c r="AZ38" s="3"/>
       <c r="BA38" s="3"/>
       <c r="BB38" s="3"/>
-      <c r="BC38" s="1"/>
+      <c r="BC38" s="3"/>
       <c r="BD38" s="1"/>
       <c r="BE38" s="1"/>
       <c r="BF38" s="1"/>
@@ -4449,8 +4485,9 @@
       <c r="BJ38" s="1"/>
       <c r="BK38" s="1"/>
       <c r="BL38" s="1"/>
-    </row>
-    <row r="39" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM38" s="1"/>
+    </row>
+    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4505,7 +4542,7 @@
       <c r="AZ39" s="3"/>
       <c r="BA39" s="3"/>
       <c r="BB39" s="3"/>
-      <c r="BC39" s="1"/>
+      <c r="BC39" s="3"/>
       <c r="BD39" s="1"/>
       <c r="BE39" s="1"/>
       <c r="BF39" s="1"/>
@@ -4515,8 +4552,9 @@
       <c r="BJ39" s="1"/>
       <c r="BK39" s="1"/>
       <c r="BL39" s="1"/>
-    </row>
-    <row r="40" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM39" s="1"/>
+    </row>
+    <row r="40" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4571,7 +4609,7 @@
       <c r="AZ40" s="3"/>
       <c r="BA40" s="3"/>
       <c r="BB40" s="3"/>
-      <c r="BC40" s="1"/>
+      <c r="BC40" s="3"/>
       <c r="BD40" s="1"/>
       <c r="BE40" s="1"/>
       <c r="BF40" s="1"/>
@@ -4581,8 +4619,9 @@
       <c r="BJ40" s="1"/>
       <c r="BK40" s="1"/>
       <c r="BL40" s="1"/>
-    </row>
-    <row r="41" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM40" s="1"/>
+    </row>
+    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -4637,7 +4676,7 @@
       <c r="AZ41" s="3"/>
       <c r="BA41" s="3"/>
       <c r="BB41" s="3"/>
-      <c r="BC41" s="1"/>
+      <c r="BC41" s="3"/>
       <c r="BD41" s="1"/>
       <c r="BE41" s="1"/>
       <c r="BF41" s="1"/>
@@ -4647,8 +4686,9 @@
       <c r="BJ41" s="1"/>
       <c r="BK41" s="1"/>
       <c r="BL41" s="1"/>
-    </row>
-    <row r="42" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM41" s="1"/>
+    </row>
+    <row r="42" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -4703,7 +4743,7 @@
       <c r="AZ42" s="3"/>
       <c r="BA42" s="3"/>
       <c r="BB42" s="3"/>
-      <c r="BC42" s="1"/>
+      <c r="BC42" s="3"/>
       <c r="BD42" s="1"/>
       <c r="BE42" s="1"/>
       <c r="BF42" s="1"/>
@@ -4713,8 +4753,9 @@
       <c r="BJ42" s="1"/>
       <c r="BK42" s="1"/>
       <c r="BL42" s="1"/>
-    </row>
-    <row r="43" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM42" s="1"/>
+    </row>
+    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -4769,7 +4810,7 @@
       <c r="AZ43" s="3"/>
       <c r="BA43" s="3"/>
       <c r="BB43" s="3"/>
-      <c r="BC43" s="1"/>
+      <c r="BC43" s="3"/>
       <c r="BD43" s="1"/>
       <c r="BE43" s="1"/>
       <c r="BF43" s="1"/>
@@ -4779,8 +4820,9 @@
       <c r="BJ43" s="1"/>
       <c r="BK43" s="1"/>
       <c r="BL43" s="1"/>
-    </row>
-    <row r="44" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM43" s="1"/>
+    </row>
+    <row r="44" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -4835,7 +4877,7 @@
       <c r="AZ44" s="3"/>
       <c r="BA44" s="3"/>
       <c r="BB44" s="3"/>
-      <c r="BC44" s="1"/>
+      <c r="BC44" s="3"/>
       <c r="BD44" s="1"/>
       <c r="BE44" s="1"/>
       <c r="BF44" s="1"/>
@@ -4845,8 +4887,9 @@
       <c r="BJ44" s="1"/>
       <c r="BK44" s="1"/>
       <c r="BL44" s="1"/>
-    </row>
-    <row r="45" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM44" s="1"/>
+    </row>
+    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -4901,7 +4944,7 @@
       <c r="AZ45" s="3"/>
       <c r="BA45" s="3"/>
       <c r="BB45" s="3"/>
-      <c r="BC45" s="1"/>
+      <c r="BC45" s="3"/>
       <c r="BD45" s="1"/>
       <c r="BE45" s="1"/>
       <c r="BF45" s="1"/>
@@ -4911,8 +4954,9 @@
       <c r="BJ45" s="1"/>
       <c r="BK45" s="1"/>
       <c r="BL45" s="1"/>
-    </row>
-    <row r="46" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM45" s="1"/>
+    </row>
+    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -4967,7 +5011,7 @@
       <c r="AZ46" s="3"/>
       <c r="BA46" s="3"/>
       <c r="BB46" s="3"/>
-      <c r="BC46" s="1"/>
+      <c r="BC46" s="3"/>
       <c r="BD46" s="1"/>
       <c r="BE46" s="1"/>
       <c r="BF46" s="1"/>
@@ -4977,8 +5021,9 @@
       <c r="BJ46" s="1"/>
       <c r="BK46" s="1"/>
       <c r="BL46" s="1"/>
-    </row>
-    <row r="47" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM46" s="1"/>
+    </row>
+    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -5033,7 +5078,7 @@
       <c r="AZ47" s="3"/>
       <c r="BA47" s="3"/>
       <c r="BB47" s="3"/>
-      <c r="BC47" s="1"/>
+      <c r="BC47" s="3"/>
       <c r="BD47" s="1"/>
       <c r="BE47" s="1"/>
       <c r="BF47" s="1"/>
@@ -5043,8 +5088,9 @@
       <c r="BJ47" s="1"/>
       <c r="BK47" s="1"/>
       <c r="BL47" s="1"/>
-    </row>
-    <row r="48" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM47" s="1"/>
+    </row>
+    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -5099,7 +5145,7 @@
       <c r="AZ48" s="3"/>
       <c r="BA48" s="3"/>
       <c r="BB48" s="3"/>
-      <c r="BC48" s="1"/>
+      <c r="BC48" s="3"/>
       <c r="BD48" s="1"/>
       <c r="BE48" s="1"/>
       <c r="BF48" s="1"/>
@@ -5109,8 +5155,9 @@
       <c r="BJ48" s="1"/>
       <c r="BK48" s="1"/>
       <c r="BL48" s="1"/>
-    </row>
-    <row r="49" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM48" s="1"/>
+    </row>
+    <row r="49" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -5165,7 +5212,7 @@
       <c r="AZ49" s="3"/>
       <c r="BA49" s="3"/>
       <c r="BB49" s="3"/>
-      <c r="BC49" s="1"/>
+      <c r="BC49" s="3"/>
       <c r="BD49" s="1"/>
       <c r="BE49" s="1"/>
       <c r="BF49" s="1"/>
@@ -5175,8 +5222,9 @@
       <c r="BJ49" s="1"/>
       <c r="BK49" s="1"/>
       <c r="BL49" s="1"/>
-    </row>
-    <row r="50" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM49" s="1"/>
+    </row>
+    <row r="50" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -5231,7 +5279,7 @@
       <c r="AZ50" s="3"/>
       <c r="BA50" s="3"/>
       <c r="BB50" s="3"/>
-      <c r="BC50" s="1"/>
+      <c r="BC50" s="3"/>
       <c r="BD50" s="1"/>
       <c r="BE50" s="1"/>
       <c r="BF50" s="1"/>
@@ -5241,8 +5289,9 @@
       <c r="BJ50" s="1"/>
       <c r="BK50" s="1"/>
       <c r="BL50" s="1"/>
-    </row>
-    <row r="51" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM50" s="1"/>
+    </row>
+    <row r="51" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5297,7 +5346,7 @@
       <c r="AZ51" s="3"/>
       <c r="BA51" s="3"/>
       <c r="BB51" s="3"/>
-      <c r="BC51" s="1"/>
+      <c r="BC51" s="3"/>
       <c r="BD51" s="1"/>
       <c r="BE51" s="1"/>
       <c r="BF51" s="1"/>
@@ -5307,8 +5356,9 @@
       <c r="BJ51" s="1"/>
       <c r="BK51" s="1"/>
       <c r="BL51" s="1"/>
-    </row>
-    <row r="52" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM51" s="1"/>
+    </row>
+    <row r="52" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5363,7 +5413,7 @@
       <c r="AZ52" s="3"/>
       <c r="BA52" s="3"/>
       <c r="BB52" s="3"/>
-      <c r="BC52" s="1"/>
+      <c r="BC52" s="3"/>
       <c r="BD52" s="1"/>
       <c r="BE52" s="1"/>
       <c r="BF52" s="1"/>
@@ -5373,8 +5423,9 @@
       <c r="BJ52" s="1"/>
       <c r="BK52" s="1"/>
       <c r="BL52" s="1"/>
-    </row>
-    <row r="53" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM52" s="1"/>
+    </row>
+    <row r="53" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5429,7 +5480,7 @@
       <c r="AZ53" s="3"/>
       <c r="BA53" s="3"/>
       <c r="BB53" s="3"/>
-      <c r="BC53" s="1"/>
+      <c r="BC53" s="3"/>
       <c r="BD53" s="1"/>
       <c r="BE53" s="1"/>
       <c r="BF53" s="1"/>
@@ -5439,8 +5490,9 @@
       <c r="BJ53" s="1"/>
       <c r="BK53" s="1"/>
       <c r="BL53" s="1"/>
-    </row>
-    <row r="54" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM53" s="1"/>
+    </row>
+    <row r="54" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -5495,7 +5547,7 @@
       <c r="AZ54" s="3"/>
       <c r="BA54" s="3"/>
       <c r="BB54" s="3"/>
-      <c r="BC54" s="1"/>
+      <c r="BC54" s="3"/>
       <c r="BD54" s="1"/>
       <c r="BE54" s="1"/>
       <c r="BF54" s="1"/>
@@ -5505,8 +5557,9 @@
       <c r="BJ54" s="1"/>
       <c r="BK54" s="1"/>
       <c r="BL54" s="1"/>
-    </row>
-    <row r="55" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM54" s="1"/>
+    </row>
+    <row r="55" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -5561,7 +5614,7 @@
       <c r="AZ55" s="3"/>
       <c r="BA55" s="3"/>
       <c r="BB55" s="3"/>
-      <c r="BC55" s="1"/>
+      <c r="BC55" s="3"/>
       <c r="BD55" s="1"/>
       <c r="BE55" s="1"/>
       <c r="BF55" s="1"/>
@@ -5571,8 +5624,9 @@
       <c r="BJ55" s="1"/>
       <c r="BK55" s="1"/>
       <c r="BL55" s="1"/>
-    </row>
-    <row r="56" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM55" s="1"/>
+    </row>
+    <row r="56" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -5627,7 +5681,7 @@
       <c r="AZ56" s="3"/>
       <c r="BA56" s="3"/>
       <c r="BB56" s="3"/>
-      <c r="BC56" s="1"/>
+      <c r="BC56" s="3"/>
       <c r="BD56" s="1"/>
       <c r="BE56" s="1"/>
       <c r="BF56" s="1"/>
@@ -5637,8 +5691,9 @@
       <c r="BJ56" s="1"/>
       <c r="BK56" s="1"/>
       <c r="BL56" s="1"/>
-    </row>
-    <row r="57" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM56" s="1"/>
+    </row>
+    <row r="57" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -5693,7 +5748,7 @@
       <c r="AZ57" s="3"/>
       <c r="BA57" s="3"/>
       <c r="BB57" s="3"/>
-      <c r="BC57" s="1"/>
+      <c r="BC57" s="3"/>
       <c r="BD57" s="1"/>
       <c r="BE57" s="1"/>
       <c r="BF57" s="1"/>
@@ -5703,8 +5758,9 @@
       <c r="BJ57" s="1"/>
       <c r="BK57" s="1"/>
       <c r="BL57" s="1"/>
-    </row>
-    <row r="58" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM57" s="1"/>
+    </row>
+    <row r="58" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -5759,7 +5815,7 @@
       <c r="AZ58" s="3"/>
       <c r="BA58" s="3"/>
       <c r="BB58" s="3"/>
-      <c r="BC58" s="1"/>
+      <c r="BC58" s="3"/>
       <c r="BD58" s="1"/>
       <c r="BE58" s="1"/>
       <c r="BF58" s="1"/>
@@ -5769,8 +5825,9 @@
       <c r="BJ58" s="1"/>
       <c r="BK58" s="1"/>
       <c r="BL58" s="1"/>
-    </row>
-    <row r="59" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM58" s="1"/>
+    </row>
+    <row r="59" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -5825,7 +5882,7 @@
       <c r="AZ59" s="3"/>
       <c r="BA59" s="3"/>
       <c r="BB59" s="3"/>
-      <c r="BC59" s="1"/>
+      <c r="BC59" s="3"/>
       <c r="BD59" s="1"/>
       <c r="BE59" s="1"/>
       <c r="BF59" s="1"/>
@@ -5835,8 +5892,9 @@
       <c r="BJ59" s="1"/>
       <c r="BK59" s="1"/>
       <c r="BL59" s="1"/>
-    </row>
-    <row r="60" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM59" s="1"/>
+    </row>
+    <row r="60" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -5891,7 +5949,7 @@
       <c r="AZ60" s="3"/>
       <c r="BA60" s="3"/>
       <c r="BB60" s="3"/>
-      <c r="BC60" s="1"/>
+      <c r="BC60" s="3"/>
       <c r="BD60" s="1"/>
       <c r="BE60" s="1"/>
       <c r="BF60" s="1"/>
@@ -5901,8 +5959,9 @@
       <c r="BJ60" s="1"/>
       <c r="BK60" s="1"/>
       <c r="BL60" s="1"/>
-    </row>
-    <row r="61" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM60" s="1"/>
+    </row>
+    <row r="61" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -5957,7 +6016,7 @@
       <c r="AZ61" s="3"/>
       <c r="BA61" s="3"/>
       <c r="BB61" s="3"/>
-      <c r="BC61" s="1"/>
+      <c r="BC61" s="3"/>
       <c r="BD61" s="1"/>
       <c r="BE61" s="1"/>
       <c r="BF61" s="1"/>
@@ -5967,8 +6026,9 @@
       <c r="BJ61" s="1"/>
       <c r="BK61" s="1"/>
       <c r="BL61" s="1"/>
-    </row>
-    <row r="62" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM61" s="1"/>
+    </row>
+    <row r="62" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -6023,7 +6083,7 @@
       <c r="AZ62" s="3"/>
       <c r="BA62" s="3"/>
       <c r="BB62" s="3"/>
-      <c r="BC62" s="1"/>
+      <c r="BC62" s="3"/>
       <c r="BD62" s="1"/>
       <c r="BE62" s="1"/>
       <c r="BF62" s="1"/>
@@ -6033,8 +6093,9 @@
       <c r="BJ62" s="1"/>
       <c r="BK62" s="1"/>
       <c r="BL62" s="1"/>
-    </row>
-    <row r="63" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM62" s="1"/>
+    </row>
+    <row r="63" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -6089,7 +6150,7 @@
       <c r="AZ63" s="3"/>
       <c r="BA63" s="3"/>
       <c r="BB63" s="3"/>
-      <c r="BC63" s="1"/>
+      <c r="BC63" s="3"/>
       <c r="BD63" s="1"/>
       <c r="BE63" s="1"/>
       <c r="BF63" s="1"/>
@@ -6099,8 +6160,9 @@
       <c r="BJ63" s="1"/>
       <c r="BK63" s="1"/>
       <c r="BL63" s="1"/>
-    </row>
-    <row r="64" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM63" s="1"/>
+    </row>
+    <row r="64" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -6155,7 +6217,7 @@
       <c r="AZ64" s="3"/>
       <c r="BA64" s="3"/>
       <c r="BB64" s="3"/>
-      <c r="BC64" s="1"/>
+      <c r="BC64" s="3"/>
       <c r="BD64" s="1"/>
       <c r="BE64" s="1"/>
       <c r="BF64" s="1"/>
@@ -6165,8 +6227,9 @@
       <c r="BJ64" s="1"/>
       <c r="BK64" s="1"/>
       <c r="BL64" s="1"/>
-    </row>
-    <row r="65" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM64" s="1"/>
+    </row>
+    <row r="65" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -6221,7 +6284,7 @@
       <c r="AZ65" s="3"/>
       <c r="BA65" s="3"/>
       <c r="BB65" s="3"/>
-      <c r="BC65" s="1"/>
+      <c r="BC65" s="3"/>
       <c r="BD65" s="1"/>
       <c r="BE65" s="1"/>
       <c r="BF65" s="1"/>
@@ -6231,8 +6294,9 @@
       <c r="BJ65" s="1"/>
       <c r="BK65" s="1"/>
       <c r="BL65" s="1"/>
-    </row>
-    <row r="66" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM65" s="1"/>
+    </row>
+    <row r="66" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -6287,7 +6351,7 @@
       <c r="AZ66" s="3"/>
       <c r="BA66" s="3"/>
       <c r="BB66" s="3"/>
-      <c r="BC66" s="1"/>
+      <c r="BC66" s="3"/>
       <c r="BD66" s="1"/>
       <c r="BE66" s="1"/>
       <c r="BF66" s="1"/>
@@ -6297,8 +6361,9 @@
       <c r="BJ66" s="1"/>
       <c r="BK66" s="1"/>
       <c r="BL66" s="1"/>
-    </row>
-    <row r="67" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM66" s="1"/>
+    </row>
+    <row r="67" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -6353,7 +6418,7 @@
       <c r="AZ67" s="3"/>
       <c r="BA67" s="3"/>
       <c r="BB67" s="3"/>
-      <c r="BC67" s="1"/>
+      <c r="BC67" s="3"/>
       <c r="BD67" s="1"/>
       <c r="BE67" s="1"/>
       <c r="BF67" s="1"/>
@@ -6363,8 +6428,9 @@
       <c r="BJ67" s="1"/>
       <c r="BK67" s="1"/>
       <c r="BL67" s="1"/>
-    </row>
-    <row r="68" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM67" s="1"/>
+    </row>
+    <row r="68" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -6419,7 +6485,7 @@
       <c r="AZ68" s="3"/>
       <c r="BA68" s="3"/>
       <c r="BB68" s="3"/>
-      <c r="BC68" s="1"/>
+      <c r="BC68" s="3"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="1"/>
       <c r="BF68" s="1"/>
@@ -6429,8 +6495,9 @@
       <c r="BJ68" s="1"/>
       <c r="BK68" s="1"/>
       <c r="BL68" s="1"/>
-    </row>
-    <row r="69" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM68" s="1"/>
+    </row>
+    <row r="69" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -6485,7 +6552,7 @@
       <c r="AZ69" s="3"/>
       <c r="BA69" s="3"/>
       <c r="BB69" s="3"/>
-      <c r="BC69" s="1"/>
+      <c r="BC69" s="3"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="1"/>
       <c r="BF69" s="1"/>
@@ -6495,8 +6562,9 @@
       <c r="BJ69" s="1"/>
       <c r="BK69" s="1"/>
       <c r="BL69" s="1"/>
-    </row>
-    <row r="70" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM69" s="1"/>
+    </row>
+    <row r="70" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -6551,7 +6619,7 @@
       <c r="AZ70" s="3"/>
       <c r="BA70" s="3"/>
       <c r="BB70" s="3"/>
-      <c r="BC70" s="1"/>
+      <c r="BC70" s="3"/>
       <c r="BD70" s="1"/>
       <c r="BE70" s="1"/>
       <c r="BF70" s="1"/>
@@ -6561,8 +6629,9 @@
       <c r="BJ70" s="1"/>
       <c r="BK70" s="1"/>
       <c r="BL70" s="1"/>
-    </row>
-    <row r="71" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM70" s="1"/>
+    </row>
+    <row r="71" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -6617,7 +6686,7 @@
       <c r="AZ71" s="3"/>
       <c r="BA71" s="3"/>
       <c r="BB71" s="3"/>
-      <c r="BC71" s="1"/>
+      <c r="BC71" s="3"/>
       <c r="BD71" s="1"/>
       <c r="BE71" s="1"/>
       <c r="BF71" s="1"/>
@@ -6627,8 +6696,9 @@
       <c r="BJ71" s="1"/>
       <c r="BK71" s="1"/>
       <c r="BL71" s="1"/>
-    </row>
-    <row r="72" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM71" s="1"/>
+    </row>
+    <row r="72" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -6683,7 +6753,7 @@
       <c r="AZ72" s="3"/>
       <c r="BA72" s="3"/>
       <c r="BB72" s="3"/>
-      <c r="BC72" s="1"/>
+      <c r="BC72" s="3"/>
       <c r="BD72" s="1"/>
       <c r="BE72" s="1"/>
       <c r="BF72" s="1"/>
@@ -6693,8 +6763,9 @@
       <c r="BJ72" s="1"/>
       <c r="BK72" s="1"/>
       <c r="BL72" s="1"/>
-    </row>
-    <row r="73" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM72" s="1"/>
+    </row>
+    <row r="73" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -6749,7 +6820,7 @@
       <c r="AZ73" s="3"/>
       <c r="BA73" s="3"/>
       <c r="BB73" s="3"/>
-      <c r="BC73" s="1"/>
+      <c r="BC73" s="3"/>
       <c r="BD73" s="1"/>
       <c r="BE73" s="1"/>
       <c r="BF73" s="1"/>
@@ -6759,8 +6830,9 @@
       <c r="BJ73" s="1"/>
       <c r="BK73" s="1"/>
       <c r="BL73" s="1"/>
-    </row>
-    <row r="74" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM73" s="1"/>
+    </row>
+    <row r="74" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -6815,7 +6887,7 @@
       <c r="AZ74" s="3"/>
       <c r="BA74" s="3"/>
       <c r="BB74" s="3"/>
-      <c r="BC74" s="1"/>
+      <c r="BC74" s="3"/>
       <c r="BD74" s="1"/>
       <c r="BE74" s="1"/>
       <c r="BF74" s="1"/>
@@ -6825,8 +6897,9 @@
       <c r="BJ74" s="1"/>
       <c r="BK74" s="1"/>
       <c r="BL74" s="1"/>
-    </row>
-    <row r="75" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM74" s="1"/>
+    </row>
+    <row r="75" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -6881,7 +6954,7 @@
       <c r="AZ75" s="3"/>
       <c r="BA75" s="3"/>
       <c r="BB75" s="3"/>
-      <c r="BC75" s="1"/>
+      <c r="BC75" s="3"/>
       <c r="BD75" s="1"/>
       <c r="BE75" s="1"/>
       <c r="BF75" s="1"/>
@@ -6891,8 +6964,9 @@
       <c r="BJ75" s="1"/>
       <c r="BK75" s="1"/>
       <c r="BL75" s="1"/>
-    </row>
-    <row r="76" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM75" s="1"/>
+    </row>
+    <row r="76" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -6947,7 +7021,7 @@
       <c r="AZ76" s="3"/>
       <c r="BA76" s="3"/>
       <c r="BB76" s="3"/>
-      <c r="BC76" s="1"/>
+      <c r="BC76" s="3"/>
       <c r="BD76" s="1"/>
       <c r="BE76" s="1"/>
       <c r="BF76" s="1"/>
@@ -6957,8 +7031,9 @@
       <c r="BJ76" s="1"/>
       <c r="BK76" s="1"/>
       <c r="BL76" s="1"/>
-    </row>
-    <row r="77" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM76" s="1"/>
+    </row>
+    <row r="77" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -7013,7 +7088,7 @@
       <c r="AZ77" s="3"/>
       <c r="BA77" s="3"/>
       <c r="BB77" s="3"/>
-      <c r="BC77" s="1"/>
+      <c r="BC77" s="3"/>
       <c r="BD77" s="1"/>
       <c r="BE77" s="1"/>
       <c r="BF77" s="1"/>
@@ -7023,8 +7098,9 @@
       <c r="BJ77" s="1"/>
       <c r="BK77" s="1"/>
       <c r="BL77" s="1"/>
-    </row>
-    <row r="78" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM77" s="1"/>
+    </row>
+    <row r="78" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -7079,7 +7155,7 @@
       <c r="AZ78" s="3"/>
       <c r="BA78" s="3"/>
       <c r="BB78" s="3"/>
-      <c r="BC78" s="1"/>
+      <c r="BC78" s="3"/>
       <c r="BD78" s="1"/>
       <c r="BE78" s="1"/>
       <c r="BF78" s="1"/>
@@ -7089,8 +7165,9 @@
       <c r="BJ78" s="1"/>
       <c r="BK78" s="1"/>
       <c r="BL78" s="1"/>
-    </row>
-    <row r="79" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM78" s="1"/>
+    </row>
+    <row r="79" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -7145,7 +7222,7 @@
       <c r="AZ79" s="3"/>
       <c r="BA79" s="3"/>
       <c r="BB79" s="3"/>
-      <c r="BC79" s="1"/>
+      <c r="BC79" s="3"/>
       <c r="BD79" s="1"/>
       <c r="BE79" s="1"/>
       <c r="BF79" s="1"/>
@@ -7155,8 +7232,9 @@
       <c r="BJ79" s="1"/>
       <c r="BK79" s="1"/>
       <c r="BL79" s="1"/>
-    </row>
-    <row r="80" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM79" s="1"/>
+    </row>
+    <row r="80" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -7211,7 +7289,7 @@
       <c r="AZ80" s="3"/>
       <c r="BA80" s="3"/>
       <c r="BB80" s="3"/>
-      <c r="BC80" s="1"/>
+      <c r="BC80" s="3"/>
       <c r="BD80" s="1"/>
       <c r="BE80" s="1"/>
       <c r="BF80" s="1"/>
@@ -7221,8 +7299,9 @@
       <c r="BJ80" s="1"/>
       <c r="BK80" s="1"/>
       <c r="BL80" s="1"/>
-    </row>
-    <row r="81" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM80" s="1"/>
+    </row>
+    <row r="81" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -7277,7 +7356,7 @@
       <c r="AZ81" s="3"/>
       <c r="BA81" s="3"/>
       <c r="BB81" s="3"/>
-      <c r="BC81" s="1"/>
+      <c r="BC81" s="3"/>
       <c r="BD81" s="1"/>
       <c r="BE81" s="1"/>
       <c r="BF81" s="1"/>
@@ -7287,8 +7366,9 @@
       <c r="BJ81" s="1"/>
       <c r="BK81" s="1"/>
       <c r="BL81" s="1"/>
-    </row>
-    <row r="82" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM81" s="1"/>
+    </row>
+    <row r="82" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -7343,7 +7423,7 @@
       <c r="AZ82" s="3"/>
       <c r="BA82" s="3"/>
       <c r="BB82" s="3"/>
-      <c r="BC82" s="1"/>
+      <c r="BC82" s="3"/>
       <c r="BD82" s="1"/>
       <c r="BE82" s="1"/>
       <c r="BF82" s="1"/>
@@ -7353,8 +7433,9 @@
       <c r="BJ82" s="1"/>
       <c r="BK82" s="1"/>
       <c r="BL82" s="1"/>
-    </row>
-    <row r="83" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM82" s="1"/>
+    </row>
+    <row r="83" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -7409,7 +7490,7 @@
       <c r="AZ83" s="3"/>
       <c r="BA83" s="3"/>
       <c r="BB83" s="3"/>
-      <c r="BC83" s="1"/>
+      <c r="BC83" s="3"/>
       <c r="BD83" s="1"/>
       <c r="BE83" s="1"/>
       <c r="BF83" s="1"/>
@@ -7419,8 +7500,9 @@
       <c r="BJ83" s="1"/>
       <c r="BK83" s="1"/>
       <c r="BL83" s="1"/>
-    </row>
-    <row r="84" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM83" s="1"/>
+    </row>
+    <row r="84" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -7475,7 +7557,7 @@
       <c r="AZ84" s="3"/>
       <c r="BA84" s="3"/>
       <c r="BB84" s="3"/>
-      <c r="BC84" s="1"/>
+      <c r="BC84" s="3"/>
       <c r="BD84" s="1"/>
       <c r="BE84" s="1"/>
       <c r="BF84" s="1"/>
@@ -7485,8 +7567,9 @@
       <c r="BJ84" s="1"/>
       <c r="BK84" s="1"/>
       <c r="BL84" s="1"/>
-    </row>
-    <row r="85" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM84" s="1"/>
+    </row>
+    <row r="85" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -7541,7 +7624,7 @@
       <c r="AZ85" s="3"/>
       <c r="BA85" s="3"/>
       <c r="BB85" s="3"/>
-      <c r="BC85" s="1"/>
+      <c r="BC85" s="3"/>
       <c r="BD85" s="1"/>
       <c r="BE85" s="1"/>
       <c r="BF85" s="1"/>
@@ -7551,8 +7634,9 @@
       <c r="BJ85" s="1"/>
       <c r="BK85" s="1"/>
       <c r="BL85" s="1"/>
-    </row>
-    <row r="86" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM85" s="1"/>
+    </row>
+    <row r="86" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -7607,7 +7691,7 @@
       <c r="AZ86" s="3"/>
       <c r="BA86" s="3"/>
       <c r="BB86" s="3"/>
-      <c r="BC86" s="1"/>
+      <c r="BC86" s="3"/>
       <c r="BD86" s="1"/>
       <c r="BE86" s="1"/>
       <c r="BF86" s="1"/>
@@ -7617,8 +7701,9 @@
       <c r="BJ86" s="1"/>
       <c r="BK86" s="1"/>
       <c r="BL86" s="1"/>
-    </row>
-    <row r="87" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM86" s="1"/>
+    </row>
+    <row r="87" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -7673,7 +7758,7 @@
       <c r="AZ87" s="3"/>
       <c r="BA87" s="3"/>
       <c r="BB87" s="3"/>
-      <c r="BC87" s="1"/>
+      <c r="BC87" s="3"/>
       <c r="BD87" s="1"/>
       <c r="BE87" s="1"/>
       <c r="BF87" s="1"/>
@@ -7683,8 +7768,9 @@
       <c r="BJ87" s="1"/>
       <c r="BK87" s="1"/>
       <c r="BL87" s="1"/>
-    </row>
-    <row r="88" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM87" s="1"/>
+    </row>
+    <row r="88" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -7739,7 +7825,7 @@
       <c r="AZ88" s="3"/>
       <c r="BA88" s="3"/>
       <c r="BB88" s="3"/>
-      <c r="BC88" s="1"/>
+      <c r="BC88" s="3"/>
       <c r="BD88" s="1"/>
       <c r="BE88" s="1"/>
       <c r="BF88" s="1"/>
@@ -7749,8 +7835,9 @@
       <c r="BJ88" s="1"/>
       <c r="BK88" s="1"/>
       <c r="BL88" s="1"/>
-    </row>
-    <row r="89" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM88" s="1"/>
+    </row>
+    <row r="89" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -7805,7 +7892,7 @@
       <c r="AZ89" s="3"/>
       <c r="BA89" s="3"/>
       <c r="BB89" s="3"/>
-      <c r="BC89" s="1"/>
+      <c r="BC89" s="3"/>
       <c r="BD89" s="1"/>
       <c r="BE89" s="1"/>
       <c r="BF89" s="1"/>
@@ -7815,8 +7902,9 @@
       <c r="BJ89" s="1"/>
       <c r="BK89" s="1"/>
       <c r="BL89" s="1"/>
-    </row>
-    <row r="90" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM89" s="1"/>
+    </row>
+    <row r="90" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -7871,7 +7959,7 @@
       <c r="AZ90" s="3"/>
       <c r="BA90" s="3"/>
       <c r="BB90" s="3"/>
-      <c r="BC90" s="1"/>
+      <c r="BC90" s="3"/>
       <c r="BD90" s="1"/>
       <c r="BE90" s="1"/>
       <c r="BF90" s="1"/>
@@ -7881,8 +7969,9 @@
       <c r="BJ90" s="1"/>
       <c r="BK90" s="1"/>
       <c r="BL90" s="1"/>
-    </row>
-    <row r="91" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM90" s="1"/>
+    </row>
+    <row r="91" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -7937,7 +8026,7 @@
       <c r="AZ91" s="3"/>
       <c r="BA91" s="3"/>
       <c r="BB91" s="3"/>
-      <c r="BC91" s="1"/>
+      <c r="BC91" s="3"/>
       <c r="BD91" s="1"/>
       <c r="BE91" s="1"/>
       <c r="BF91" s="1"/>
@@ -7947,8 +8036,9 @@
       <c r="BJ91" s="1"/>
       <c r="BK91" s="1"/>
       <c r="BL91" s="1"/>
-    </row>
-    <row r="92" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM91" s="1"/>
+    </row>
+    <row r="92" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -8003,7 +8093,7 @@
       <c r="AZ92" s="3"/>
       <c r="BA92" s="3"/>
       <c r="BB92" s="3"/>
-      <c r="BC92" s="1"/>
+      <c r="BC92" s="3"/>
       <c r="BD92" s="1"/>
       <c r="BE92" s="1"/>
       <c r="BF92" s="1"/>
@@ -8013,8 +8103,9 @@
       <c r="BJ92" s="1"/>
       <c r="BK92" s="1"/>
       <c r="BL92" s="1"/>
-    </row>
-    <row r="93" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM92" s="1"/>
+    </row>
+    <row r="93" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -8069,7 +8160,7 @@
       <c r="AZ93" s="3"/>
       <c r="BA93" s="3"/>
       <c r="BB93" s="3"/>
-      <c r="BC93" s="1"/>
+      <c r="BC93" s="3"/>
       <c r="BD93" s="1"/>
       <c r="BE93" s="1"/>
       <c r="BF93" s="1"/>
@@ -8079,8 +8170,9 @@
       <c r="BJ93" s="1"/>
       <c r="BK93" s="1"/>
       <c r="BL93" s="1"/>
-    </row>
-    <row r="94" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM93" s="1"/>
+    </row>
+    <row r="94" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -8135,7 +8227,7 @@
       <c r="AZ94" s="3"/>
       <c r="BA94" s="3"/>
       <c r="BB94" s="3"/>
-      <c r="BC94" s="1"/>
+      <c r="BC94" s="3"/>
       <c r="BD94" s="1"/>
       <c r="BE94" s="1"/>
       <c r="BF94" s="1"/>
@@ -8145,8 +8237,9 @@
       <c r="BJ94" s="1"/>
       <c r="BK94" s="1"/>
       <c r="BL94" s="1"/>
-    </row>
-    <row r="95" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM94" s="1"/>
+    </row>
+    <row r="95" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -8201,7 +8294,7 @@
       <c r="AZ95" s="3"/>
       <c r="BA95" s="3"/>
       <c r="BB95" s="3"/>
-      <c r="BC95" s="1"/>
+      <c r="BC95" s="3"/>
       <c r="BD95" s="1"/>
       <c r="BE95" s="1"/>
       <c r="BF95" s="1"/>
@@ -8211,8 +8304,9 @@
       <c r="BJ95" s="1"/>
       <c r="BK95" s="1"/>
       <c r="BL95" s="1"/>
-    </row>
-    <row r="96" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM95" s="1"/>
+    </row>
+    <row r="96" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -8267,8 +8361,9 @@
       <c r="AZ96" s="2"/>
       <c r="BA96" s="2"/>
       <c r="BB96" s="2"/>
-    </row>
-    <row r="97" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC96" s="2"/>
+    </row>
+    <row r="97" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -8323,8 +8418,9 @@
       <c r="AZ97" s="2"/>
       <c r="BA97" s="2"/>
       <c r="BB97" s="2"/>
-    </row>
-    <row r="98" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC97" s="2"/>
+    </row>
+    <row r="98" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -8379,8 +8475,9 @@
       <c r="AZ98" s="2"/>
       <c r="BA98" s="2"/>
       <c r="BB98" s="2"/>
-    </row>
-    <row r="99" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC98" s="2"/>
+    </row>
+    <row r="99" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -8435,8 +8532,9 @@
       <c r="AZ99" s="2"/>
       <c r="BA99" s="2"/>
       <c r="BB99" s="2"/>
-    </row>
-    <row r="100" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC99" s="2"/>
+    </row>
+    <row r="100" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -8491,8 +8589,9 @@
       <c r="AZ100" s="2"/>
       <c r="BA100" s="2"/>
       <c r="BB100" s="2"/>
-    </row>
-    <row r="101" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC100" s="2"/>
+    </row>
+    <row r="101" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -8547,8 +8646,9 @@
       <c r="AZ101" s="2"/>
       <c r="BA101" s="2"/>
       <c r="BB101" s="2"/>
-    </row>
-    <row r="102" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC101" s="2"/>
+    </row>
+    <row r="102" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -8603,8 +8703,9 @@
       <c r="AZ102" s="2"/>
       <c r="BA102" s="2"/>
       <c r="BB102" s="2"/>
-    </row>
-    <row r="103" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC102" s="2"/>
+    </row>
+    <row r="103" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -8659,8 +8760,9 @@
       <c r="AZ103" s="2"/>
       <c r="BA103" s="2"/>
       <c r="BB103" s="2"/>
-    </row>
-    <row r="104" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC103" s="2"/>
+    </row>
+    <row r="104" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -8715,8 +8817,9 @@
       <c r="AZ104" s="2"/>
       <c r="BA104" s="2"/>
       <c r="BB104" s="2"/>
-    </row>
-    <row r="105" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC104" s="2"/>
+    </row>
+    <row r="105" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -8771,8 +8874,9 @@
       <c r="AZ105" s="2"/>
       <c r="BA105" s="2"/>
       <c r="BB105" s="2"/>
-    </row>
-    <row r="106" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC105" s="2"/>
+    </row>
+    <row r="106" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -8827,29 +8931,31 @@
       <c r="AZ106" s="2"/>
       <c r="BA106" s="2"/>
       <c r="BB106" s="2"/>
+      <c r="BC106" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="O2:Z2"/>
+    <mergeCell ref="AZ1:AZ3"/>
+    <mergeCell ref="AA2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="O1:AQ1"/>
+    <mergeCell ref="AR1:AY1"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="AV2:AY2"/>
+    <mergeCell ref="AP2:AP3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Y2"/>
-    <mergeCell ref="AY1:AY3"/>
-    <mergeCell ref="Z2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="N1:AP1"/>
-    <mergeCell ref="AQ1:AX1"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Presentation and folder with the stuff to send
Former-commit-id: 39234ae3c4e1de79bbdc94d5b3a72fce4fa44cb2
</commit_message>
<xml_diff>
--- a/result_report.xlsx
+++ b/result_report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>Version</t>
   </si>
@@ -240,12 +240,6 @@
   </si>
   <si>
     <t>Op/sec</t>
-  </si>
-  <si>
-    <t>division</t>
-  </si>
-  <si>
-    <t>Balanced Synthesis</t>
   </si>
   <si>
     <t>r4</t>
@@ -789,7 +783,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -978,17 +972,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1017,21 +1019,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1338,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS107"/>
+  <dimension ref="A1:BS106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BF7" sqref="BF7"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,74 +1362,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="78" t="s">
+      <c r="G1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="72" t="s">
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
-      <c r="AK1" s="72"/>
-      <c r="AL1" s="72"/>
-      <c r="AM1" s="72"/>
-      <c r="AN1" s="72"/>
-      <c r="AO1" s="72"/>
-      <c r="AP1" s="72"/>
-      <c r="AQ1" s="72"/>
-      <c r="AR1" s="72"/>
-      <c r="AS1" s="72"/>
-      <c r="AT1" s="72"/>
-      <c r="AU1" s="72"/>
-      <c r="AV1" s="72"/>
-      <c r="AW1" s="72"/>
-      <c r="AX1" s="73" t="s">
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="74"/>
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="74"/>
+      <c r="AF1" s="74"/>
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="74"/>
+      <c r="AI1" s="74"/>
+      <c r="AJ1" s="74"/>
+      <c r="AK1" s="74"/>
+      <c r="AL1" s="74"/>
+      <c r="AM1" s="74"/>
+      <c r="AN1" s="74"/>
+      <c r="AO1" s="74"/>
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="74"/>
+      <c r="AR1" s="74"/>
+      <c r="AS1" s="74"/>
+      <c r="AT1" s="74"/>
+      <c r="AU1" s="74"/>
+      <c r="AV1" s="74"/>
+      <c r="AW1" s="74"/>
+      <c r="AX1" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="AY1" s="73"/>
-      <c r="AZ1" s="73"/>
-      <c r="BA1" s="73"/>
-      <c r="BB1" s="73"/>
-      <c r="BC1" s="73"/>
-      <c r="BD1" s="73"/>
-      <c r="BE1" s="73"/>
-      <c r="BF1" s="67" t="s">
+      <c r="AY1" s="75"/>
+      <c r="AZ1" s="75"/>
+      <c r="BA1" s="75"/>
+      <c r="BB1" s="75"/>
+      <c r="BC1" s="75"/>
+      <c r="BD1" s="75"/>
+      <c r="BE1" s="75"/>
+      <c r="BF1" s="70" t="s">
         <v>41</v>
       </c>
       <c r="BG1" s="3"/>
@@ -1460,92 +1447,92 @@
       <c r="BS1" s="1"/>
     </row>
     <row r="2" spans="1:71" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
-      <c r="B2" s="68" t="s">
+      <c r="A2" s="66"/>
+      <c r="B2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68" t="s">
+      <c r="E2" s="69"/>
+      <c r="F2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68" t="s">
+      <c r="J2" s="69"/>
+      <c r="K2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68" t="s">
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="68"/>
-      <c r="Y2" s="68"/>
-      <c r="Z2" s="68"/>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="68" t="s">
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="69"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="AC2" s="68"/>
-      <c r="AD2" s="68"/>
-      <c r="AE2" s="68"/>
-      <c r="AF2" s="68"/>
-      <c r="AG2" s="68"/>
-      <c r="AH2" s="68"/>
-      <c r="AI2" s="68"/>
-      <c r="AJ2" s="68"/>
-      <c r="AK2" s="68"/>
-      <c r="AL2" s="68" t="s">
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="69"/>
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="69"/>
+      <c r="AK2" s="69"/>
+      <c r="AL2" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="AM2" s="68"/>
-      <c r="AN2" s="68"/>
-      <c r="AO2" s="68"/>
-      <c r="AP2" s="68"/>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="68" t="s">
+      <c r="AM2" s="69"/>
+      <c r="AN2" s="69"/>
+      <c r="AO2" s="69"/>
+      <c r="AP2" s="69"/>
+      <c r="AQ2" s="76"/>
+      <c r="AR2" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="AS2" s="77" t="s">
+      <c r="AS2" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="AT2" s="77"/>
-      <c r="AU2" s="68" t="s">
+      <c r="AT2" s="79"/>
+      <c r="AU2" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="AV2" s="68"/>
-      <c r="AW2" s="69" t="s">
+      <c r="AV2" s="69"/>
+      <c r="AW2" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="AX2" s="74" t="s">
+      <c r="AX2" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="AY2" s="75"/>
-      <c r="AZ2" s="75"/>
-      <c r="BA2" s="76"/>
-      <c r="BB2" s="74" t="s">
+      <c r="AY2" s="77"/>
+      <c r="AZ2" s="77"/>
+      <c r="BA2" s="78"/>
+      <c r="BB2" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="BC2" s="75"/>
-      <c r="BD2" s="75"/>
-      <c r="BE2" s="76"/>
-      <c r="BF2" s="67"/>
+      <c r="BC2" s="77"/>
+      <c r="BD2" s="77"/>
+      <c r="BE2" s="78"/>
+      <c r="BF2" s="70"/>
       <c r="BG2" s="3"/>
       <c r="BH2" s="3"/>
       <c r="BI2" s="3"/>
@@ -1561,61 +1548,61 @@
       <c r="BS2" s="1"/>
     </row>
     <row r="3" spans="1:71" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
-      <c r="X3" s="68"/>
-      <c r="Y3" s="68"/>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
-      <c r="AJ3" s="68"/>
-      <c r="AK3" s="68"/>
-      <c r="AL3" s="68" t="s">
+      <c r="A3" s="66"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="69"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="69"/>
+      <c r="AB3" s="69"/>
+      <c r="AC3" s="69"/>
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="69"/>
+      <c r="AF3" s="69"/>
+      <c r="AG3" s="69"/>
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="69"/>
+      <c r="AJ3" s="69"/>
+      <c r="AK3" s="69"/>
+      <c r="AL3" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68" t="s">
+      <c r="AM3" s="69"/>
+      <c r="AN3" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68" t="s">
+      <c r="AO3" s="69"/>
+      <c r="AP3" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="AQ3" s="74"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="77"/>
-      <c r="AT3" s="77"/>
-      <c r="AU3" s="68"/>
-      <c r="AV3" s="68"/>
-      <c r="AW3" s="70"/>
+      <c r="AQ3" s="76"/>
+      <c r="AR3" s="69"/>
+      <c r="AS3" s="79"/>
+      <c r="AT3" s="79"/>
+      <c r="AU3" s="69"/>
+      <c r="AV3" s="69"/>
+      <c r="AW3" s="72"/>
       <c r="AX3" s="46"/>
       <c r="AY3" s="47"/>
       <c r="AZ3" s="47"/>
@@ -1624,7 +1611,7 @@
       <c r="BC3" s="47"/>
       <c r="BD3" s="47"/>
       <c r="BE3" s="48"/>
-      <c r="BF3" s="67"/>
+      <c r="BF3" s="70"/>
       <c r="BG3" s="3"/>
       <c r="BH3" s="3"/>
       <c r="BI3" s="3"/>
@@ -1640,7 +1627,7 @@
       <c r="BS3" s="1"/>
     </row>
     <row r="4" spans="1:71" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
@@ -1653,10 +1640,10 @@
       <c r="E4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="82"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="15" t="s">
         <v>11</v>
       </c>
@@ -1765,7 +1752,7 @@
       <c r="AQ4" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="AR4" s="68"/>
+      <c r="AR4" s="69"/>
       <c r="AS4" s="57" t="s">
         <v>50</v>
       </c>
@@ -1778,7 +1765,7 @@
       <c r="AV4" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="AW4" s="71"/>
+      <c r="AW4" s="73"/>
       <c r="AX4" s="35" t="s">
         <v>57</v>
       </c>
@@ -1803,7 +1790,7 @@
       <c r="BE4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="BF4" s="67"/>
+      <c r="BF4" s="70"/>
       <c r="BG4" s="3"/>
       <c r="BH4" s="3"/>
       <c r="BI4" s="3"/>
@@ -1970,7 +1957,7 @@
         <v>219.28</v>
       </c>
       <c r="AX5" s="38">
-        <f t="shared" ref="AX5:AX13" si="0">I5+J5</f>
+        <f t="shared" ref="AX5:AX12" si="0">I5+J5</f>
         <v>26793</v>
       </c>
       <c r="AY5" s="39">
@@ -1978,7 +1965,7 @@
         <v>1.2418966245249744E-2</v>
       </c>
       <c r="AZ5" s="39">
-        <f t="shared" ref="AZ5:AZ13" si="1">M5</f>
+        <f t="shared" ref="AZ5:AZ12" si="1">M5</f>
         <v>3.1880000000000002</v>
       </c>
       <c r="BA5" s="39">
@@ -2016,492 +2003,392 @@
       <c r="BR5" s="1"/>
       <c r="BS5" s="1"/>
     </row>
-    <row r="6" spans="1:71" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:71" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="12">
+        <v>19</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="10">
-        <v>19</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="33">
-        <v>80.340999999999994</v>
-      </c>
-      <c r="G6" s="33">
+      <c r="F6" s="12">
+        <v>80.534999999999997</v>
+      </c>
+      <c r="G6" s="32">
         <v>106.32899999999999</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="12">
         <v>80</v>
       </c>
-      <c r="I6" s="10">
-        <v>10478</v>
-      </c>
-      <c r="J6" s="10">
-        <v>17866</v>
-      </c>
-      <c r="K6" s="58">
+      <c r="I6" s="12">
+        <v>10479</v>
+      </c>
+      <c r="J6" s="12">
+        <v>17865</v>
+      </c>
+      <c r="K6" s="59">
         <v>2.468</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="12">
         <v>0.74299999999999999</v>
       </c>
-      <c r="M6" s="10">
-        <v>3.2120000000000002</v>
+      <c r="M6" s="12">
+        <v>3.2109999999999999</v>
       </c>
       <c r="N6" s="45">
-        <f t="shared" ref="N6:N8" si="2">M6/F6</f>
-        <v>3.9979587010368307E-2</v>
-      </c>
-      <c r="O6" s="29">
+        <f t="shared" ref="N6:N7" si="2">M6/F6</f>
+        <v>3.9870863599677162E-2</v>
+      </c>
+      <c r="O6" s="30">
         <v>100</v>
       </c>
-      <c r="P6" s="29">
-        <v>116</v>
-      </c>
-      <c r="Q6" s="29">
-        <v>67</v>
-      </c>
-      <c r="R6" s="29">
-        <v>100</v>
-      </c>
-      <c r="S6" s="29">
+      <c r="P6" s="30">
+        <v>117</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>83</v>
+      </c>
+      <c r="R6" s="30">
+        <v>84</v>
+      </c>
+      <c r="S6" s="30">
         <v>800</v>
       </c>
-      <c r="T6" s="29">
-        <v>733</v>
-      </c>
-      <c r="U6" s="29">
-        <v>84</v>
-      </c>
-      <c r="V6" s="29">
-        <v>133</v>
-      </c>
-      <c r="W6" s="29">
-        <v>450</v>
-      </c>
-      <c r="X6" s="29">
+      <c r="T6" s="30">
+        <v>717</v>
+      </c>
+      <c r="U6" s="30">
+        <v>83</v>
+      </c>
+      <c r="V6" s="30">
+        <v>150</v>
+      </c>
+      <c r="W6" s="30">
+        <v>434</v>
+      </c>
+      <c r="X6" s="30">
         <v>1150</v>
       </c>
-      <c r="Y6" s="29">
-        <v>259</v>
-      </c>
-      <c r="Z6" s="29">
-        <v>1003</v>
-      </c>
-      <c r="AA6" s="26">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="AB6" s="33">
+      <c r="Y6" s="30">
+        <v>257</v>
+      </c>
+      <c r="Z6" s="30">
+        <v>1002</v>
+      </c>
+      <c r="AA6" s="25">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AB6" s="32">
         <v>0.45400000000000001</v>
       </c>
-      <c r="AC6" s="33">
+      <c r="AC6" s="32">
         <v>0.29099999999999998</v>
       </c>
-      <c r="AD6" s="33">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="AE6" s="33">
+      <c r="AD6" s="32">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="AE6" s="32">
         <v>0.246</v>
       </c>
-      <c r="AF6" s="33">
+      <c r="AF6" s="32">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AG6" s="33">
+      <c r="AG6" s="32">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AH6" s="33">
+      <c r="AH6" s="32">
         <v>1.6579999999999999</v>
       </c>
-      <c r="AI6" s="33">
+      <c r="AI6" s="32">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AJ6" s="33">
+      <c r="AJ6" s="32">
         <v>2.3839999999999999</v>
       </c>
-      <c r="AK6" s="33">
-        <f>60+53.22</f>
-        <v>113.22</v>
-      </c>
-      <c r="AL6" s="29">
-        <v>800</v>
-      </c>
-      <c r="AM6" s="26">
-        <v>13.14</v>
-      </c>
-      <c r="AN6" s="29">
-        <v>16335</v>
-      </c>
-      <c r="AO6" s="26">
-        <v>10.54</v>
-      </c>
-      <c r="AP6" s="29">
-        <v>5284</v>
-      </c>
-      <c r="AQ6" s="26">
-        <v>10.51</v>
-      </c>
-      <c r="AR6" s="26">
-        <v>7.66</v>
-      </c>
-      <c r="AS6" s="26">
-        <v>24.41</v>
-      </c>
-      <c r="AT6" s="26">
-        <v>20.3</v>
-      </c>
-      <c r="AU6" s="29">
-        <v>7345</v>
-      </c>
-      <c r="AV6" s="26">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="AW6" s="26">
-        <f>3*60+33.06</f>
-        <v>213.06</v>
-      </c>
-      <c r="AX6" s="38">
-        <f t="shared" ref="AX6:AX7" si="3">I6+J6</f>
-        <v>28344</v>
-      </c>
-      <c r="AY6" s="39">
-        <f t="shared" ref="AY6:AY7" si="4">1/F6</f>
-        <v>1.244694489737494E-2</v>
-      </c>
-      <c r="AZ6" s="39">
-        <f t="shared" ref="AZ6:AZ7" si="5">M6</f>
-        <v>3.2120000000000002</v>
-      </c>
-      <c r="BA6" s="39">
-        <f t="shared" ref="BA6:BA7" si="6">AW6</f>
-        <v>213.06</v>
-      </c>
-      <c r="BB6" s="38">
-        <f t="shared" ref="BB6:BB7" si="7">AX6*AY6</f>
-        <v>352.79620617119531</v>
-      </c>
-      <c r="BC6" s="39">
-        <f t="shared" ref="BC6:BC7" si="8">AX6*BA6</f>
-        <v>6038972.6399999997</v>
-      </c>
-      <c r="BD6" s="39">
-        <f t="shared" ref="BD6:BD7" si="9">AZ6*AY6</f>
-        <v>3.9979587010368307E-2</v>
-      </c>
-      <c r="BE6" s="41">
-        <f t="shared" ref="BE6:BE7" si="10">AZ6*BA6</f>
-        <v>684.34872000000007</v>
-      </c>
-      <c r="BF6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="BG6" s="64"/>
-      <c r="BH6" s="64"/>
-      <c r="BI6" s="64"/>
-      <c r="BJ6" s="65"/>
-      <c r="BK6" s="65"/>
-      <c r="BL6" s="65"/>
-      <c r="BM6" s="65"/>
-      <c r="BN6" s="65"/>
-      <c r="BO6" s="65"/>
-      <c r="BP6" s="65"/>
-      <c r="BQ6" s="65"/>
-      <c r="BR6" s="65"/>
-      <c r="BS6" s="65"/>
-    </row>
-    <row r="7" spans="1:71" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="12">
-        <v>80.534999999999997</v>
-      </c>
-      <c r="G7" s="32">
-        <v>106.32899999999999</v>
-      </c>
-      <c r="H7" s="12">
-        <v>80</v>
-      </c>
-      <c r="I7" s="12">
-        <v>10479</v>
-      </c>
-      <c r="J7" s="12">
-        <v>17865</v>
-      </c>
-      <c r="K7" s="59">
-        <v>2.468</v>
-      </c>
-      <c r="L7" s="12">
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="M7" s="12">
-        <v>3.2109999999999999</v>
-      </c>
-      <c r="N7" s="45">
-        <f t="shared" si="2"/>
-        <v>3.9870863599677162E-2</v>
-      </c>
-      <c r="O7" s="30">
-        <v>100</v>
-      </c>
-      <c r="P7" s="30">
-        <v>117</v>
-      </c>
-      <c r="Q7" s="30">
-        <v>83</v>
-      </c>
-      <c r="R7" s="30">
-        <v>84</v>
-      </c>
-      <c r="S7" s="30">
-        <v>800</v>
-      </c>
-      <c r="T7" s="30">
-        <v>717</v>
-      </c>
-      <c r="U7" s="30">
-        <v>83</v>
-      </c>
-      <c r="V7" s="30">
-        <v>150</v>
-      </c>
-      <c r="W7" s="30">
-        <v>434</v>
-      </c>
-      <c r="X7" s="30">
-        <v>1150</v>
-      </c>
-      <c r="Y7" s="30">
-        <v>257</v>
-      </c>
-      <c r="Z7" s="30">
-        <v>1002</v>
-      </c>
-      <c r="AA7" s="25">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="AB7" s="32">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="AC7" s="32">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="AD7" s="32">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="AE7" s="32">
-        <v>0.246</v>
-      </c>
-      <c r="AF7" s="32">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AG7" s="32">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AH7" s="32">
-        <v>1.6579999999999999</v>
-      </c>
-      <c r="AI7" s="32">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AJ7" s="32">
-        <v>2.3839999999999999</v>
-      </c>
-      <c r="AK7" s="32">
+      <c r="AK6" s="32">
         <f>60+53.25</f>
         <v>113.25</v>
       </c>
-      <c r="AL7" s="30">
+      <c r="AL6" s="30">
         <v>801</v>
       </c>
-      <c r="AM7" s="25">
+      <c r="AM6" s="25">
         <v>13.13</v>
       </c>
-      <c r="AN7" s="30">
+      <c r="AN6" s="30">
         <v>16335</v>
       </c>
-      <c r="AO7" s="25">
+      <c r="AO6" s="25">
         <v>10.53</v>
       </c>
-      <c r="AP7" s="30">
+      <c r="AP6" s="30">
         <v>5284</v>
       </c>
-      <c r="AQ7" s="25">
+      <c r="AQ6" s="25">
         <v>10.5</v>
       </c>
-      <c r="AR7" s="25">
+      <c r="AR6" s="25">
         <v>7.65</v>
       </c>
-      <c r="AS7" s="25">
+      <c r="AS6" s="25">
         <v>24.31</v>
       </c>
-      <c r="AT7" s="25">
+      <c r="AT6" s="25">
         <v>20.62</v>
       </c>
-      <c r="AU7" s="30">
+      <c r="AU6" s="30">
         <v>7345</v>
       </c>
-      <c r="AV7" s="25">
+      <c r="AV6" s="25">
         <v>10.210000000000001</v>
       </c>
-      <c r="AW7" s="25">
+      <c r="AW6" s="25">
         <f>3*60+33.3</f>
         <v>213.3</v>
       </c>
-      <c r="AX7" s="38">
-        <f t="shared" si="3"/>
+      <c r="AX6" s="38">
+        <f t="shared" ref="AX6" si="3">I6+J6</f>
         <v>28344</v>
       </c>
-      <c r="AY7" s="39">
-        <f t="shared" si="4"/>
+      <c r="AY6" s="39">
+        <f t="shared" ref="AY6" si="4">1/F6</f>
         <v>1.2416961569503943E-2</v>
       </c>
-      <c r="AZ7" s="39">
-        <f t="shared" si="5"/>
+      <c r="AZ6" s="39">
+        <f t="shared" ref="AZ6" si="5">M6</f>
         <v>3.2109999999999999</v>
       </c>
-      <c r="BA7" s="39">
-        <f t="shared" si="6"/>
+      <c r="BA6" s="39">
+        <f t="shared" ref="BA6" si="6">AW6</f>
         <v>213.3</v>
       </c>
-      <c r="BB7" s="38">
-        <f t="shared" si="7"/>
+      <c r="BB6" s="38">
+        <f t="shared" ref="BB6" si="7">AX6*AY6</f>
         <v>351.94635872601975</v>
       </c>
-      <c r="BC7" s="39">
-        <f t="shared" si="8"/>
+      <c r="BC6" s="39">
+        <f t="shared" ref="BC6" si="8">AX6*BA6</f>
         <v>6045775.2000000002</v>
       </c>
-      <c r="BD7" s="39">
-        <f t="shared" si="9"/>
+      <c r="BD6" s="39">
+        <f t="shared" ref="BD6" si="9">AZ6*AY6</f>
         <v>3.9870863599677162E-2</v>
       </c>
-      <c r="BE7" s="41">
-        <f t="shared" si="10"/>
+      <c r="BE6" s="41">
+        <f t="shared" ref="BE6" si="10">AZ6*BA6</f>
         <v>684.90629999999999</v>
       </c>
-      <c r="BF7" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="BG7" s="61"/>
-      <c r="BH7" s="61"/>
-      <c r="BI7" s="61"/>
-      <c r="BJ7" s="62"/>
-      <c r="BK7" s="62"/>
-      <c r="BL7" s="62"/>
-      <c r="BM7" s="62"/>
-      <c r="BN7" s="62"/>
-      <c r="BO7" s="62"/>
-      <c r="BP7" s="62"/>
-      <c r="BQ7" s="62"/>
-      <c r="BR7" s="62"/>
-      <c r="BS7" s="62"/>
-    </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="45" t="e">
+      <c r="BF6" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG6" s="61"/>
+      <c r="BH6" s="61"/>
+      <c r="BI6" s="61"/>
+      <c r="BJ6" s="62"/>
+      <c r="BK6" s="62"/>
+      <c r="BL6" s="62"/>
+      <c r="BM6" s="62"/>
+      <c r="BN6" s="62"/>
+      <c r="BO6" s="62"/>
+      <c r="BP6" s="62"/>
+      <c r="BQ6" s="62"/>
+      <c r="BR6" s="62"/>
+      <c r="BS6" s="62"/>
+    </row>
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="45" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="29"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="33"/>
-      <c r="AC8" s="33"/>
-      <c r="AD8" s="33"/>
-      <c r="AE8" s="33"/>
-      <c r="AF8" s="33"/>
-      <c r="AG8" s="33"/>
-      <c r="AH8" s="33"/>
-      <c r="AI8" s="33"/>
-      <c r="AJ8" s="33"/>
-      <c r="AK8" s="33"/>
-      <c r="AL8" s="29"/>
-      <c r="AM8" s="26"/>
-      <c r="AN8" s="29"/>
-      <c r="AO8" s="26"/>
-      <c r="AP8" s="29"/>
-      <c r="AQ8" s="26"/>
-      <c r="AR8" s="26"/>
-      <c r="AS8" s="26"/>
-      <c r="AT8" s="26"/>
-      <c r="AU8" s="29"/>
-      <c r="AV8" s="26"/>
-      <c r="AW8" s="26"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="33"/>
+      <c r="AC7" s="33"/>
+      <c r="AD7" s="33"/>
+      <c r="AE7" s="33"/>
+      <c r="AF7" s="33"/>
+      <c r="AG7" s="33"/>
+      <c r="AH7" s="33"/>
+      <c r="AI7" s="33"/>
+      <c r="AJ7" s="33"/>
+      <c r="AK7" s="33"/>
+      <c r="AL7" s="29"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="29"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="29"/>
+      <c r="AQ7" s="26"/>
+      <c r="AR7" s="26"/>
+      <c r="AS7" s="26"/>
+      <c r="AT7" s="26"/>
+      <c r="AU7" s="29"/>
+      <c r="AV7" s="26"/>
+      <c r="AW7" s="26"/>
+      <c r="AX7" s="38">
+        <f t="shared" ref="AX7" si="11">I7+J7</f>
+        <v>0</v>
+      </c>
+      <c r="AY7" s="39" t="e">
+        <f t="shared" ref="AY7" si="12">1/F7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AZ7" s="39">
+        <f t="shared" ref="AZ7" si="13">M7</f>
+        <v>0</v>
+      </c>
+      <c r="BA7" s="39">
+        <f t="shared" ref="BA7" si="14">AW7</f>
+        <v>0</v>
+      </c>
+      <c r="BB7" s="38" t="e">
+        <f t="shared" ref="BB7" si="15">AX7*AY7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC7" s="39">
+        <f t="shared" ref="BC7" si="16">AX7*BA7</f>
+        <v>0</v>
+      </c>
+      <c r="BD7" s="39" t="e">
+        <f t="shared" ref="BD7" si="17">AZ7*AY7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BE7" s="41">
+        <f t="shared" ref="BE7" si="18">AZ7*BA7</f>
+        <v>0</v>
+      </c>
+      <c r="BF7" s="21"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
+      <c r="BI7" s="3"/>
+      <c r="BJ7" s="1"/>
+      <c r="BK7" s="1"/>
+      <c r="BL7" s="1"/>
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+      <c r="BO7" s="1"/>
+      <c r="BP7" s="1"/>
+      <c r="BQ7" s="1"/>
+      <c r="BR7" s="1"/>
+      <c r="BS7" s="1"/>
+    </row>
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="45" t="e">
+        <f t="shared" ref="N8:N12" si="19">M8/F8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="30"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
+      <c r="AI8" s="32"/>
+      <c r="AJ8" s="32"/>
+      <c r="AK8" s="32"/>
+      <c r="AL8" s="32"/>
+      <c r="AM8" s="25"/>
+      <c r="AN8" s="30"/>
+      <c r="AO8" s="25"/>
+      <c r="AP8" s="30"/>
+      <c r="AQ8" s="25"/>
+      <c r="AR8" s="25"/>
+      <c r="AS8" s="25"/>
+      <c r="AT8" s="25"/>
+      <c r="AU8" s="30"/>
+      <c r="AV8" s="25"/>
+      <c r="AW8" s="25"/>
       <c r="AX8" s="38">
-        <f t="shared" ref="AX8" si="11">I8+J8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AY8" s="39" t="e">
-        <f t="shared" ref="AY8" si="12">1/F8</f>
+        <f t="shared" ref="AY8:AY12" si="20">1/F8</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AZ8" s="39">
-        <f t="shared" ref="AZ8" si="13">M8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BA8" s="39">
-        <f t="shared" ref="BA8" si="14">AW8</f>
+        <f t="shared" ref="BA8:BA12" si="21">AW8</f>
         <v>0</v>
       </c>
       <c r="BB8" s="38" t="e">
-        <f t="shared" ref="BB8" si="15">AX8*AY8</f>
+        <f t="shared" ref="BB8:BB12" si="22">AX8*AY8</f>
         <v>#DIV/0!</v>
       </c>
       <c r="BC8" s="39">
-        <f t="shared" ref="BC8" si="16">AX8*BA8</f>
+        <f t="shared" ref="BC8:BC12" si="23">AX8*BA8</f>
         <v>0</v>
       </c>
       <c r="BD8" s="39" t="e">
-        <f t="shared" ref="BD8" si="17">AZ8*AY8</f>
+        <f t="shared" ref="BD8:BD12" si="24">AZ8*AY8</f>
         <v>#DIV/0!</v>
       </c>
       <c r="BE8" s="41">
-        <f t="shared" ref="BE8" si="18">AZ8*BA8</f>
+        <f t="shared" ref="BE8:BE12" si="25">AZ8*BA8</f>
         <v>0</v>
       </c>
-      <c r="BF8" s="21"/>
+      <c r="BF8" s="22"/>
       <c r="BG8" s="3"/>
       <c r="BH8" s="3"/>
       <c r="BI8" s="3"/>
@@ -2517,64 +2404,64 @@
       <c r="BS8" s="1"/>
     </row>
     <row r="9" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="45" t="e">
-        <f t="shared" ref="N9:N13" si="19">M9/F9</f>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="32"/>
-      <c r="AC9" s="32"/>
-      <c r="AD9" s="32"/>
-      <c r="AE9" s="32"/>
-      <c r="AF9" s="32"/>
-      <c r="AG9" s="32"/>
-      <c r="AH9" s="32"/>
-      <c r="AI9" s="32"/>
-      <c r="AJ9" s="32"/>
-      <c r="AK9" s="32"/>
-      <c r="AL9" s="32"/>
-      <c r="AM9" s="25"/>
-      <c r="AN9" s="30"/>
-      <c r="AO9" s="25"/>
-      <c r="AP9" s="30"/>
-      <c r="AQ9" s="25"/>
-      <c r="AR9" s="25"/>
-      <c r="AS9" s="25"/>
-      <c r="AT9" s="25"/>
-      <c r="AU9" s="30"/>
-      <c r="AV9" s="25"/>
-      <c r="AW9" s="25"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="33"/>
+      <c r="AC9" s="33"/>
+      <c r="AD9" s="33"/>
+      <c r="AE9" s="33"/>
+      <c r="AF9" s="33"/>
+      <c r="AG9" s="33"/>
+      <c r="AH9" s="33"/>
+      <c r="AI9" s="33"/>
+      <c r="AJ9" s="33"/>
+      <c r="AK9" s="33"/>
+      <c r="AL9" s="33"/>
+      <c r="AM9" s="26"/>
+      <c r="AN9" s="29"/>
+      <c r="AO9" s="26"/>
+      <c r="AP9" s="29"/>
+      <c r="AQ9" s="26"/>
+      <c r="AR9" s="26"/>
+      <c r="AS9" s="26"/>
+      <c r="AT9" s="26"/>
+      <c r="AU9" s="29"/>
+      <c r="AV9" s="26"/>
+      <c r="AW9" s="26"/>
       <c r="AX9" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AY9" s="39" t="e">
-        <f t="shared" ref="AY9:AY13" si="20">1/F9</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AZ9" s="39">
@@ -2582,26 +2469,26 @@
         <v>0</v>
       </c>
       <c r="BA9" s="39">
-        <f t="shared" ref="BA9:BA13" si="21">AW9</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="BB9" s="38" t="e">
-        <f t="shared" ref="BB9:BB13" si="22">AX9*AY9</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BC9" s="39">
-        <f t="shared" ref="BC9:BC13" si="23">AX9*BA9</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="BD9" s="39" t="e">
-        <f t="shared" ref="BD9:BD13" si="24">AZ9*AY9</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BE9" s="41">
-        <f t="shared" ref="BE9:BE13" si="25">AZ9*BA9</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BF9" s="22"/>
+      <c r="BF9" s="21"/>
       <c r="BG9" s="3"/>
       <c r="BH9" s="3"/>
       <c r="BI9" s="3"/>
@@ -2617,58 +2504,58 @@
       <c r="BS9" s="1"/>
     </row>
     <row r="10" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
       <c r="N10" s="45" t="e">
         <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="33"/>
-      <c r="AC10" s="33"/>
-      <c r="AD10" s="33"/>
-      <c r="AE10" s="33"/>
-      <c r="AF10" s="33"/>
-      <c r="AG10" s="33"/>
-      <c r="AH10" s="33"/>
-      <c r="AI10" s="33"/>
-      <c r="AJ10" s="33"/>
-      <c r="AK10" s="33"/>
-      <c r="AL10" s="33"/>
-      <c r="AM10" s="26"/>
-      <c r="AN10" s="29"/>
-      <c r="AO10" s="26"/>
-      <c r="AP10" s="29"/>
-      <c r="AQ10" s="26"/>
-      <c r="AR10" s="26"/>
-      <c r="AS10" s="26"/>
-      <c r="AT10" s="26"/>
-      <c r="AU10" s="29"/>
-      <c r="AV10" s="26"/>
-      <c r="AW10" s="26"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="32"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="32"/>
+      <c r="AF10" s="32"/>
+      <c r="AG10" s="32"/>
+      <c r="AH10" s="32"/>
+      <c r="AI10" s="32"/>
+      <c r="AJ10" s="32"/>
+      <c r="AK10" s="32"/>
+      <c r="AL10" s="32"/>
+      <c r="AM10" s="25"/>
+      <c r="AN10" s="30"/>
+      <c r="AO10" s="25"/>
+      <c r="AP10" s="30"/>
+      <c r="AQ10" s="25"/>
+      <c r="AR10" s="25"/>
+      <c r="AS10" s="25"/>
+      <c r="AT10" s="25"/>
+      <c r="AU10" s="30"/>
+      <c r="AV10" s="25"/>
+      <c r="AW10" s="25"/>
       <c r="AX10" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2701,7 +2588,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BF10" s="21"/>
+      <c r="BF10" s="22"/>
       <c r="BG10" s="3"/>
       <c r="BH10" s="3"/>
       <c r="BI10" s="3"/>
@@ -2717,58 +2604,58 @@
       <c r="BS10" s="1"/>
     </row>
     <row r="11" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
       <c r="N11" s="45" t="e">
         <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="30"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="32"/>
-      <c r="AC11" s="32"/>
-      <c r="AD11" s="32"/>
-      <c r="AE11" s="32"/>
-      <c r="AF11" s="32"/>
-      <c r="AG11" s="32"/>
-      <c r="AH11" s="32"/>
-      <c r="AI11" s="32"/>
-      <c r="AJ11" s="32"/>
-      <c r="AK11" s="32"/>
-      <c r="AL11" s="32"/>
-      <c r="AM11" s="25"/>
-      <c r="AN11" s="30"/>
-      <c r="AO11" s="25"/>
-      <c r="AP11" s="30"/>
-      <c r="AQ11" s="25"/>
-      <c r="AR11" s="25"/>
-      <c r="AS11" s="25"/>
-      <c r="AT11" s="25"/>
-      <c r="AU11" s="30"/>
-      <c r="AV11" s="25"/>
-      <c r="AW11" s="25"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="33"/>
+      <c r="AF11" s="33"/>
+      <c r="AG11" s="33"/>
+      <c r="AH11" s="33"/>
+      <c r="AI11" s="33"/>
+      <c r="AJ11" s="33"/>
+      <c r="AK11" s="33"/>
+      <c r="AL11" s="33"/>
+      <c r="AM11" s="26"/>
+      <c r="AN11" s="29"/>
+      <c r="AO11" s="26"/>
+      <c r="AP11" s="29"/>
+      <c r="AQ11" s="26"/>
+      <c r="AR11" s="26"/>
+      <c r="AS11" s="26"/>
+      <c r="AT11" s="26"/>
+      <c r="AU11" s="29"/>
+      <c r="AV11" s="26"/>
+      <c r="AW11" s="26"/>
       <c r="AX11" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2801,7 +2688,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BF11" s="22"/>
+      <c r="BF11" s="21"/>
       <c r="BG11" s="3"/>
       <c r="BH11" s="3"/>
       <c r="BI11" s="3"/>
@@ -2817,91 +2704,91 @@
       <c r="BS11" s="1"/>
     </row>
     <row r="12" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
       <c r="N12" s="45" t="e">
         <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="33"/>
-      <c r="AC12" s="33"/>
-      <c r="AD12" s="33"/>
-      <c r="AE12" s="33"/>
-      <c r="AF12" s="33"/>
-      <c r="AG12" s="33"/>
-      <c r="AH12" s="33"/>
-      <c r="AI12" s="33"/>
-      <c r="AJ12" s="33"/>
-      <c r="AK12" s="33"/>
-      <c r="AL12" s="33"/>
-      <c r="AM12" s="26"/>
-      <c r="AN12" s="29"/>
-      <c r="AO12" s="26"/>
-      <c r="AP12" s="29"/>
-      <c r="AQ12" s="26"/>
-      <c r="AR12" s="26"/>
-      <c r="AS12" s="26"/>
-      <c r="AT12" s="26"/>
-      <c r="AU12" s="29"/>
-      <c r="AV12" s="26"/>
-      <c r="AW12" s="26"/>
-      <c r="AX12" s="38">
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="49"/>
+      <c r="AG12" s="49"/>
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="49"/>
+      <c r="AJ12" s="49"/>
+      <c r="AK12" s="49"/>
+      <c r="AL12" s="49"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="27"/>
+      <c r="AP12" s="50"/>
+      <c r="AQ12" s="27"/>
+      <c r="AR12" s="27"/>
+      <c r="AS12" s="27"/>
+      <c r="AT12" s="27"/>
+      <c r="AU12" s="50"/>
+      <c r="AV12" s="27"/>
+      <c r="AW12" s="27"/>
+      <c r="AX12" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AY12" s="39" t="e">
+      <c r="AY12" s="43" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AZ12" s="39">
+      <c r="AZ12" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BA12" s="39">
+      <c r="BA12" s="43">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="BB12" s="38" t="e">
+      <c r="BB12" s="42" t="e">
         <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BC12" s="39">
+      <c r="BC12" s="43">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="BD12" s="39" t="e">
+      <c r="BD12" s="43" t="e">
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BE12" s="41">
+      <c r="BE12" s="44">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BF12" s="21"/>
+      <c r="BF12" s="23"/>
       <c r="BG12" s="3"/>
       <c r="BH12" s="3"/>
       <c r="BI12" s="3"/>
@@ -2917,91 +2804,64 @@
       <c r="BS12" s="1"/>
     </row>
     <row r="13" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="45" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="50"/>
-      <c r="Z13" s="50"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="49"/>
-      <c r="AC13" s="49"/>
-      <c r="AD13" s="49"/>
-      <c r="AE13" s="49"/>
-      <c r="AF13" s="49"/>
-      <c r="AG13" s="49"/>
-      <c r="AH13" s="49"/>
-      <c r="AI13" s="49"/>
-      <c r="AJ13" s="49"/>
-      <c r="AK13" s="49"/>
-      <c r="AL13" s="49"/>
-      <c r="AM13" s="27"/>
-      <c r="AN13" s="50"/>
-      <c r="AO13" s="27"/>
-      <c r="AP13" s="50"/>
-      <c r="AQ13" s="27"/>
-      <c r="AR13" s="27"/>
-      <c r="AS13" s="27"/>
-      <c r="AT13" s="27"/>
-      <c r="AU13" s="50"/>
-      <c r="AV13" s="27"/>
-      <c r="AW13" s="27"/>
-      <c r="AX13" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AY13" s="43" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ13" s="43">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BA13" s="43">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="BB13" s="42" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC13" s="43">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="BD13" s="43" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BE13" s="44">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="BF13" s="23"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AT13" s="3"/>
+      <c r="AU13" s="3"/>
+      <c r="AV13" s="3"/>
+      <c r="AW13" s="3"/>
+      <c r="AX13" s="3"/>
+      <c r="AY13" s="3"/>
+      <c r="AZ13" s="3"/>
+      <c r="BA13" s="3"/>
+      <c r="BB13" s="3"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
       <c r="BG13" s="3"/>
       <c r="BH13" s="3"/>
       <c r="BI13" s="3"/>
@@ -9003,77 +8863,67 @@
       <c r="BS95" s="1"/>
     </row>
     <row r="96" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-      <c r="Q96" s="3"/>
-      <c r="R96" s="3"/>
-      <c r="S96" s="3"/>
-      <c r="T96" s="3"/>
-      <c r="U96" s="3"/>
-      <c r="V96" s="3"/>
-      <c r="W96" s="3"/>
-      <c r="X96" s="3"/>
-      <c r="Y96" s="3"/>
-      <c r="Z96" s="3"/>
-      <c r="AA96" s="3"/>
-      <c r="AB96" s="3"/>
-      <c r="AC96" s="3"/>
-      <c r="AD96" s="3"/>
-      <c r="AE96" s="3"/>
-      <c r="AF96" s="3"/>
-      <c r="AG96" s="3"/>
-      <c r="AH96" s="3"/>
-      <c r="AI96" s="3"/>
-      <c r="AJ96" s="3"/>
-      <c r="AK96" s="3"/>
-      <c r="AL96" s="3"/>
-      <c r="AM96" s="3"/>
-      <c r="AN96" s="3"/>
-      <c r="AO96" s="3"/>
-      <c r="AP96" s="3"/>
-      <c r="AQ96" s="3"/>
-      <c r="AR96" s="3"/>
-      <c r="AS96" s="3"/>
-      <c r="AT96" s="3"/>
-      <c r="AU96" s="3"/>
-      <c r="AV96" s="3"/>
-      <c r="AW96" s="3"/>
-      <c r="AX96" s="3"/>
-      <c r="AY96" s="3"/>
-      <c r="AZ96" s="3"/>
-      <c r="BA96" s="3"/>
-      <c r="BB96" s="3"/>
-      <c r="BC96" s="3"/>
-      <c r="BD96" s="3"/>
-      <c r="BE96" s="3"/>
-      <c r="BF96" s="3"/>
-      <c r="BG96" s="3"/>
-      <c r="BH96" s="3"/>
-      <c r="BI96" s="3"/>
-      <c r="BJ96" s="1"/>
-      <c r="BK96" s="1"/>
-      <c r="BL96" s="1"/>
-      <c r="BM96" s="1"/>
-      <c r="BN96" s="1"/>
-      <c r="BO96" s="1"/>
-      <c r="BP96" s="1"/>
-      <c r="BQ96" s="1"/>
-      <c r="BR96" s="1"/>
-      <c r="BS96" s="1"/>
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
+      <c r="P96" s="2"/>
+      <c r="Q96" s="2"/>
+      <c r="R96" s="2"/>
+      <c r="S96" s="2"/>
+      <c r="T96" s="2"/>
+      <c r="U96" s="2"/>
+      <c r="V96" s="2"/>
+      <c r="W96" s="2"/>
+      <c r="X96" s="2"/>
+      <c r="Y96" s="2"/>
+      <c r="Z96" s="2"/>
+      <c r="AA96" s="2"/>
+      <c r="AB96" s="2"/>
+      <c r="AC96" s="2"/>
+      <c r="AD96" s="2"/>
+      <c r="AE96" s="2"/>
+      <c r="AF96" s="2"/>
+      <c r="AG96" s="2"/>
+      <c r="AH96" s="2"/>
+      <c r="AI96" s="2"/>
+      <c r="AJ96" s="2"/>
+      <c r="AK96" s="2"/>
+      <c r="AL96" s="2"/>
+      <c r="AM96" s="2"/>
+      <c r="AN96" s="2"/>
+      <c r="AO96" s="2"/>
+      <c r="AP96" s="2"/>
+      <c r="AQ96" s="2"/>
+      <c r="AR96" s="2"/>
+      <c r="AS96" s="2"/>
+      <c r="AT96" s="2"/>
+      <c r="AU96" s="2"/>
+      <c r="AV96" s="2"/>
+      <c r="AW96" s="2"/>
+      <c r="AX96" s="2"/>
+      <c r="AY96" s="2"/>
+      <c r="AZ96" s="2"/>
+      <c r="BA96" s="2"/>
+      <c r="BB96" s="2"/>
+      <c r="BC96" s="2"/>
+      <c r="BD96" s="2"/>
+      <c r="BE96" s="2"/>
+      <c r="BF96" s="2"/>
+      <c r="BG96" s="2"/>
+      <c r="BH96" s="2"/>
+      <c r="BI96" s="2"/>
     </row>
     <row r="97" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
@@ -9705,80 +9555,8 @@
       <c r="BH106" s="2"/>
       <c r="BI106" s="2"/>
     </row>
-    <row r="107" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
-      <c r="N107" s="2"/>
-      <c r="O107" s="2"/>
-      <c r="P107" s="2"/>
-      <c r="Q107" s="2"/>
-      <c r="R107" s="2"/>
-      <c r="S107" s="2"/>
-      <c r="T107" s="2"/>
-      <c r="U107" s="2"/>
-      <c r="V107" s="2"/>
-      <c r="W107" s="2"/>
-      <c r="X107" s="2"/>
-      <c r="Y107" s="2"/>
-      <c r="Z107" s="2"/>
-      <c r="AA107" s="2"/>
-      <c r="AB107" s="2"/>
-      <c r="AC107" s="2"/>
-      <c r="AD107" s="2"/>
-      <c r="AE107" s="2"/>
-      <c r="AF107" s="2"/>
-      <c r="AG107" s="2"/>
-      <c r="AH107" s="2"/>
-      <c r="AI107" s="2"/>
-      <c r="AJ107" s="2"/>
-      <c r="AK107" s="2"/>
-      <c r="AL107" s="2"/>
-      <c r="AM107" s="2"/>
-      <c r="AN107" s="2"/>
-      <c r="AO107" s="2"/>
-      <c r="AP107" s="2"/>
-      <c r="AQ107" s="2"/>
-      <c r="AR107" s="2"/>
-      <c r="AS107" s="2"/>
-      <c r="AT107" s="2"/>
-      <c r="AU107" s="2"/>
-      <c r="AV107" s="2"/>
-      <c r="AW107" s="2"/>
-      <c r="AX107" s="2"/>
-      <c r="AY107" s="2"/>
-      <c r="AZ107" s="2"/>
-      <c r="BA107" s="2"/>
-      <c r="BB107" s="2"/>
-      <c r="BC107" s="2"/>
-      <c r="BD107" s="2"/>
-      <c r="BE107" s="2"/>
-      <c r="BF107" s="2"/>
-      <c r="BG107" s="2"/>
-      <c r="BH107" s="2"/>
-      <c r="BI107" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="F2:H3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="K2:N3"/>
     <mergeCell ref="BF1:BF4"/>
     <mergeCell ref="AR2:AR4"/>
     <mergeCell ref="AW2:AW4"/>
@@ -9794,6 +9572,15 @@
     <mergeCell ref="AL2:AQ2"/>
     <mergeCell ref="AS2:AT3"/>
     <mergeCell ref="AU2:AV3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:H3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="K2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>